<commit_message>
refactor: small changes in border rendering
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56D175D-9615-A149-B59B-F5278899B840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689B5B3E-4D82-9040-828A-7D880B6B3773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="147">
   <si>
     <t>Layout Property</t>
   </si>
@@ -47,15 +47,6 @@
     <t>Theme Variable</t>
   </si>
   <si>
-    <t>horizontalAlignment</t>
-  </si>
-  <si>
-    <t>verticalAlignment</t>
-  </si>
-  <si>
-    <t>orientation</t>
-  </si>
-  <si>
     <t>width</t>
   </si>
   <si>
@@ -257,14 +248,242 @@
     <t>whiteSpace</t>
   </si>
   <si>
-    <t>Non-CSS; Check if it can be removed</t>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>min-width</t>
+  </si>
+  <si>
+    <t>max-width</t>
+  </si>
+  <si>
+    <t>We have a "max-content-width" theme variable</t>
+  </si>
+  <si>
+    <t>min-height</t>
+  </si>
+  <si>
+    <t>max-height</t>
+  </si>
+  <si>
+    <t>border-top</t>
+  </si>
+  <si>
+    <t>border-right</t>
+  </si>
+  <si>
+    <t>border-bottom</t>
+  </si>
+  <si>
+    <t>border-left</t>
+  </si>
+  <si>
+    <t>border-color</t>
+  </si>
+  <si>
+    <t>color-border</t>
+  </si>
+  <si>
+    <t>border-style</t>
+  </si>
+  <si>
+    <t>style-border</t>
+  </si>
+  <si>
+    <t>border-width</t>
+  </si>
+  <si>
+    <t>thickness-border</t>
+  </si>
+  <si>
+    <t>border-radius</t>
+  </si>
+  <si>
+    <t>border-top-left-radius</t>
+  </si>
+  <si>
+    <t>radius-start-start</t>
+  </si>
+  <si>
+    <t>We do not implement top-left, only the direction-aware start-start</t>
+  </si>
+  <si>
+    <t>border-top-right-radius</t>
+  </si>
+  <si>
+    <t>radius-start-end</t>
+  </si>
+  <si>
+    <t>We do not implement top-right, only the direction-aware start-end</t>
+  </si>
+  <si>
+    <t>border-bottom-left-radius</t>
+  </si>
+  <si>
+    <t>radius-end-start</t>
+  </si>
+  <si>
+    <t>We do not implement bottom-left, only the direction-aware end-start</t>
+  </si>
+  <si>
+    <t>border-bottom-right-radius</t>
+  </si>
+  <si>
+    <t>radius-end-end</t>
+  </si>
+  <si>
+    <t>We do not implement bottom-right, only the direction-aware end-end</t>
+  </si>
+  <si>
+    <t>padding-horizontal</t>
+  </si>
+  <si>
+    <t>padding-vertical</t>
+  </si>
+  <si>
+    <t>Sets the padding-top and padding-bottom styles</t>
+  </si>
+  <si>
+    <t>Sets the padding-left and padding-right styles</t>
+  </si>
+  <si>
+    <t>padding-top</t>
+  </si>
+  <si>
+    <t>padding-right</t>
+  </si>
+  <si>
+    <t>padding-bottom</t>
+  </si>
+  <si>
+    <t>padding-left</t>
+  </si>
+  <si>
+    <t>margin-horizontal</t>
+  </si>
+  <si>
+    <t>margin-vertical</t>
+  </si>
+  <si>
+    <t>Sets the margin-left and margin-right styles</t>
+  </si>
+  <si>
+    <t>Sets the margin-top and margin-bottom styles</t>
+  </si>
+  <si>
+    <t>margin-top</t>
+  </si>
+  <si>
+    <t>margin-right</t>
+  </si>
+  <si>
+    <t>margin-bottom</t>
+  </si>
+  <si>
+    <t>margin-left</t>
+  </si>
+  <si>
+    <t>background-color</t>
+  </si>
+  <si>
+    <t>color-bg</t>
+  </si>
+  <si>
+    <t>Do we want to use it as an alias for "color-bg"?</t>
+  </si>
+  <si>
+    <t>box-shadow</t>
+  </si>
+  <si>
+    <t>If we had such a theme variable, we used "direction"</t>
+  </si>
+  <si>
+    <t>overflow-x</t>
+  </si>
+  <si>
+    <t>overflow-y</t>
+  </si>
+  <si>
+    <t>If we had such a theme variable, we used "horizontal-overflow"</t>
+  </si>
+  <si>
+    <t>If we had such a theme variable, we used "vertical-overflow"</t>
+  </si>
+  <si>
+    <t>z-index</t>
+  </si>
+  <si>
+    <t>We do not want to expose this with any theme variable</t>
+  </si>
+  <si>
+    <t>font-family</t>
+  </si>
+  <si>
+    <t>font-size</t>
+  </si>
+  <si>
+    <t>font-weight</t>
+  </si>
+  <si>
+    <t>font-style</t>
+  </si>
+  <si>
+    <t>We use "italic" as a layout property with a boolean value. We do not support the full "font-style" CSS syntax</t>
+  </si>
+  <si>
+    <t>text-decoration</t>
+  </si>
+  <si>
+    <t>user-select</t>
+  </si>
+  <si>
+    <t>If we had such a theme variable, we used "user-select"</t>
+  </si>
+  <si>
+    <t>letter-spacing</t>
+  </si>
+  <si>
+    <t>text-transform</t>
+  </si>
+  <si>
+    <t>transform, transform-text</t>
+  </si>
+  <si>
+    <t>We use two theme variable variants</t>
+  </si>
+  <si>
+    <t>line-height</t>
+  </si>
+  <si>
+    <t>text-align</t>
+  </si>
+  <si>
+    <t>text-align-last</t>
+  </si>
+  <si>
+    <t>text-wrap</t>
+  </si>
+  <si>
+    <t>flex-wrap</t>
+  </si>
+  <si>
+    <t>We use "wrapContent" as a boolean property resulting "flex-wrap: wrap" for true and "flex-wrap: nowrap" for false</t>
+  </si>
+  <si>
+    <t>flex-shrink</t>
+  </si>
+  <si>
+    <t>We use "canShrink" as a boolean property resulting "flex-shrink: 1" for true and "flex-shrink: 0" for false</t>
+  </si>
+  <si>
+    <t>white-space</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,13 +504,67 @@
       <name val="Aptos Display"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -303,15 +576,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -644,20 +928,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1293D70B-0512-624F-91B3-17CA08CDE41F}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="87" style="1" customWidth="1"/>
+    <col min="6" max="6" width="94.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -666,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -675,32 +959,44 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>73</v>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>73</v>
+      <c r="C3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>73</v>
       </c>
@@ -709,320 +1005,810 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="C41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="B44" s="7"/>
+      <c r="C44" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C50" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="C51" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B54"/>
+      <c r="C54" t="s">
+        <v>132</v>
+      </c>
+      <c r="D54" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54"/>
+      <c r="F54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="C55" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C57" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C58" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C59" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+      <c r="C60" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+      <c r="B61" s="7"/>
+      <c r="C61" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="B62" s="7"/>
+      <c r="C62" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="B63" s="3"/>
+      <c r="C63" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B64" s="3"/>
+      <c r="C64" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+      <c r="C65" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: small changes in border rendering (#769)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56D175D-9615-A149-B59B-F5278899B840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689B5B3E-4D82-9040-828A-7D880B6B3773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="147">
   <si>
     <t>Layout Property</t>
   </si>
@@ -47,15 +47,6 @@
     <t>Theme Variable</t>
   </si>
   <si>
-    <t>horizontalAlignment</t>
-  </si>
-  <si>
-    <t>verticalAlignment</t>
-  </si>
-  <si>
-    <t>orientation</t>
-  </si>
-  <si>
     <t>width</t>
   </si>
   <si>
@@ -257,14 +248,242 @@
     <t>whiteSpace</t>
   </si>
   <si>
-    <t>Non-CSS; Check if it can be removed</t>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>min-width</t>
+  </si>
+  <si>
+    <t>max-width</t>
+  </si>
+  <si>
+    <t>We have a "max-content-width" theme variable</t>
+  </si>
+  <si>
+    <t>min-height</t>
+  </si>
+  <si>
+    <t>max-height</t>
+  </si>
+  <si>
+    <t>border-top</t>
+  </si>
+  <si>
+    <t>border-right</t>
+  </si>
+  <si>
+    <t>border-bottom</t>
+  </si>
+  <si>
+    <t>border-left</t>
+  </si>
+  <si>
+    <t>border-color</t>
+  </si>
+  <si>
+    <t>color-border</t>
+  </si>
+  <si>
+    <t>border-style</t>
+  </si>
+  <si>
+    <t>style-border</t>
+  </si>
+  <si>
+    <t>border-width</t>
+  </si>
+  <si>
+    <t>thickness-border</t>
+  </si>
+  <si>
+    <t>border-radius</t>
+  </si>
+  <si>
+    <t>border-top-left-radius</t>
+  </si>
+  <si>
+    <t>radius-start-start</t>
+  </si>
+  <si>
+    <t>We do not implement top-left, only the direction-aware start-start</t>
+  </si>
+  <si>
+    <t>border-top-right-radius</t>
+  </si>
+  <si>
+    <t>radius-start-end</t>
+  </si>
+  <si>
+    <t>We do not implement top-right, only the direction-aware start-end</t>
+  </si>
+  <si>
+    <t>border-bottom-left-radius</t>
+  </si>
+  <si>
+    <t>radius-end-start</t>
+  </si>
+  <si>
+    <t>We do not implement bottom-left, only the direction-aware end-start</t>
+  </si>
+  <si>
+    <t>border-bottom-right-radius</t>
+  </si>
+  <si>
+    <t>radius-end-end</t>
+  </si>
+  <si>
+    <t>We do not implement bottom-right, only the direction-aware end-end</t>
+  </si>
+  <si>
+    <t>padding-horizontal</t>
+  </si>
+  <si>
+    <t>padding-vertical</t>
+  </si>
+  <si>
+    <t>Sets the padding-top and padding-bottom styles</t>
+  </si>
+  <si>
+    <t>Sets the padding-left and padding-right styles</t>
+  </si>
+  <si>
+    <t>padding-top</t>
+  </si>
+  <si>
+    <t>padding-right</t>
+  </si>
+  <si>
+    <t>padding-bottom</t>
+  </si>
+  <si>
+    <t>padding-left</t>
+  </si>
+  <si>
+    <t>margin-horizontal</t>
+  </si>
+  <si>
+    <t>margin-vertical</t>
+  </si>
+  <si>
+    <t>Sets the margin-left and margin-right styles</t>
+  </si>
+  <si>
+    <t>Sets the margin-top and margin-bottom styles</t>
+  </si>
+  <si>
+    <t>margin-top</t>
+  </si>
+  <si>
+    <t>margin-right</t>
+  </si>
+  <si>
+    <t>margin-bottom</t>
+  </si>
+  <si>
+    <t>margin-left</t>
+  </si>
+  <si>
+    <t>background-color</t>
+  </si>
+  <si>
+    <t>color-bg</t>
+  </si>
+  <si>
+    <t>Do we want to use it as an alias for "color-bg"?</t>
+  </si>
+  <si>
+    <t>box-shadow</t>
+  </si>
+  <si>
+    <t>If we had such a theme variable, we used "direction"</t>
+  </si>
+  <si>
+    <t>overflow-x</t>
+  </si>
+  <si>
+    <t>overflow-y</t>
+  </si>
+  <si>
+    <t>If we had such a theme variable, we used "horizontal-overflow"</t>
+  </si>
+  <si>
+    <t>If we had such a theme variable, we used "vertical-overflow"</t>
+  </si>
+  <si>
+    <t>z-index</t>
+  </si>
+  <si>
+    <t>We do not want to expose this with any theme variable</t>
+  </si>
+  <si>
+    <t>font-family</t>
+  </si>
+  <si>
+    <t>font-size</t>
+  </si>
+  <si>
+    <t>font-weight</t>
+  </si>
+  <si>
+    <t>font-style</t>
+  </si>
+  <si>
+    <t>We use "italic" as a layout property with a boolean value. We do not support the full "font-style" CSS syntax</t>
+  </si>
+  <si>
+    <t>text-decoration</t>
+  </si>
+  <si>
+    <t>user-select</t>
+  </si>
+  <si>
+    <t>If we had such a theme variable, we used "user-select"</t>
+  </si>
+  <si>
+    <t>letter-spacing</t>
+  </si>
+  <si>
+    <t>text-transform</t>
+  </si>
+  <si>
+    <t>transform, transform-text</t>
+  </si>
+  <si>
+    <t>We use two theme variable variants</t>
+  </si>
+  <si>
+    <t>line-height</t>
+  </si>
+  <si>
+    <t>text-align</t>
+  </si>
+  <si>
+    <t>text-align-last</t>
+  </si>
+  <si>
+    <t>text-wrap</t>
+  </si>
+  <si>
+    <t>flex-wrap</t>
+  </si>
+  <si>
+    <t>We use "wrapContent" as a boolean property resulting "flex-wrap: wrap" for true and "flex-wrap: nowrap" for false</t>
+  </si>
+  <si>
+    <t>flex-shrink</t>
+  </si>
+  <si>
+    <t>We use "canShrink" as a boolean property resulting "flex-shrink: 1" for true and "flex-shrink: 0" for false</t>
+  </si>
+  <si>
+    <t>white-space</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,13 +504,67 @@
       <name val="Aptos Display"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -303,15 +576,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -644,20 +928,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1293D70B-0512-624F-91B3-17CA08CDE41F}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="87" style="1" customWidth="1"/>
+    <col min="6" max="6" width="94.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -666,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -675,32 +959,44 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>73</v>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>73</v>
+      <c r="C3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>73</v>
       </c>
@@ -709,320 +1005,810 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="C41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="B44" s="7"/>
+      <c r="C44" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C50" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="C51" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B54"/>
+      <c r="C54" t="s">
+        <v>132</v>
+      </c>
+      <c r="D54" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54"/>
+      <c r="F54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="C55" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C57" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C58" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C59" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+      <c r="C60" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+      <c r="B61" s="7"/>
+      <c r="C61" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="B62" s="7"/>
+      <c r="C62" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="B63" s="3"/>
+      <c r="C63" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B64" s="3"/>
+      <c r="C64" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+      <c r="C65" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip: update theme tables
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689B5B3E-4D82-9040-828A-7D880B6B3773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465A2C25-AD4B-854D-92E5-3BB0FA4D7011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="202">
   <si>
     <t>Layout Property</t>
   </si>
@@ -305,36 +306,24 @@
     <t>radius-start-start</t>
   </si>
   <si>
-    <t>We do not implement top-left, only the direction-aware start-start</t>
-  </si>
-  <si>
     <t>border-top-right-radius</t>
   </si>
   <si>
     <t>radius-start-end</t>
   </si>
   <si>
-    <t>We do not implement top-right, only the direction-aware start-end</t>
-  </si>
-  <si>
     <t>border-bottom-left-radius</t>
   </si>
   <si>
     <t>radius-end-start</t>
   </si>
   <si>
-    <t>We do not implement bottom-left, only the direction-aware end-start</t>
-  </si>
-  <si>
     <t>border-bottom-right-radius</t>
   </si>
   <si>
     <t>radius-end-end</t>
   </si>
   <si>
-    <t>We do not implement bottom-right, only the direction-aware end-end</t>
-  </si>
-  <si>
     <t>padding-horizontal</t>
   </si>
   <si>
@@ -477,13 +466,190 @@
   </si>
   <si>
     <t>white-space</t>
+  </si>
+  <si>
+    <t>maxWidth-content</t>
+  </si>
+  <si>
+    <t>We do not use these theme variables yet. Nonetheless, they may be used in the future</t>
+  </si>
+  <si>
+    <t>borderHorizontal</t>
+  </si>
+  <si>
+    <t>borderVertical</t>
+  </si>
+  <si>
+    <t>borderRadius</t>
+  </si>
+  <si>
+    <t>borderRadiusStartStart</t>
+  </si>
+  <si>
+    <t>borderRadiusStartEnd</t>
+  </si>
+  <si>
+    <t>borderRadiusEndStart</t>
+  </si>
+  <si>
+    <t>borderRadiusEndEnd</t>
+  </si>
+  <si>
+    <t>borderWidth</t>
+  </si>
+  <si>
+    <t>paddingHorizontal</t>
+  </si>
+  <si>
+    <t>paddingVertical</t>
+  </si>
+  <si>
+    <t>marginHorizontal</t>
+  </si>
+  <si>
+    <t>marginVertical</t>
+  </si>
+  <si>
+    <t>boxShadow</t>
+  </si>
+  <si>
+    <t>overflowX</t>
+  </si>
+  <si>
+    <t>overflowY</t>
+  </si>
+  <si>
+    <t>fontStyle</t>
+  </si>
+  <si>
+    <t>transformText</t>
+  </si>
+  <si>
+    <t>scroll-padding-block-Pages</t>
+  </si>
+  <si>
+    <t>scrollPaddingBlock-Pages</t>
+  </si>
+  <si>
+    <t>Special theme variable</t>
+  </si>
+  <si>
+    <t>New name</t>
+  </si>
+  <si>
+    <t>logo-AppHeader</t>
+  </si>
+  <si>
+    <t>align-content-AppHeader</t>
+  </si>
+  <si>
+    <t>justifyContent-AppHeader</t>
+  </si>
+  <si>
+    <t>thickness-outline</t>
+  </si>
+  <si>
+    <t>outlineWidth</t>
+  </si>
+  <si>
+    <t>color-outline</t>
+  </si>
+  <si>
+    <t>outlineColor</t>
+  </si>
+  <si>
+    <t>style-outline</t>
+  </si>
+  <si>
+    <t>outlineStyle</t>
+  </si>
+  <si>
+    <t>offset-outline</t>
+  </si>
+  <si>
+    <t>outlineOffset</t>
+  </si>
+  <si>
+    <t>textDecorationLine</t>
+  </si>
+  <si>
+    <t>textDecorationColor</t>
+  </si>
+  <si>
+    <t>textDecorationStyle</t>
+  </si>
+  <si>
+    <t>textDecorationThickness</t>
+  </si>
+  <si>
+    <t>text-decoration-line</t>
+  </si>
+  <si>
+    <t>text-decoration-color</t>
+  </si>
+  <si>
+    <t>text-decoration-style</t>
+  </si>
+  <si>
+    <t>text-decoration-thickness</t>
+  </si>
+  <si>
+    <t>textUnderlineOffset</t>
+  </si>
+  <si>
+    <t>text-underline-offset</t>
+  </si>
+  <si>
+    <t>outline-width</t>
+  </si>
+  <si>
+    <t>outline-color</t>
+  </si>
+  <si>
+    <t>line-decoration</t>
+  </si>
+  <si>
+    <t>color-decoration</t>
+  </si>
+  <si>
+    <t>style-decoration</t>
+  </si>
+  <si>
+    <t>thickness-decoration</t>
+  </si>
+  <si>
+    <t>offset-decoration</t>
+  </si>
+  <si>
+    <t>width-outline</t>
+  </si>
+  <si>
+    <t>outline-style</t>
+  </si>
+  <si>
+    <t>writing-mode</t>
+  </si>
+  <si>
+    <t>Review Text (put to layout context, along with direction)</t>
+  </si>
+  <si>
+    <t>align-items</t>
+  </si>
+  <si>
+    <t>alignItems</t>
+  </si>
+  <si>
+    <t>align-content</t>
+  </si>
+  <si>
+    <t>alignContent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -506,13 +672,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF9C0006"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -527,12 +686,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Display"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF9C0006"/>
       <name val="Aptos Display"/>
       <scheme val="major"/>
@@ -542,6 +695,13 @@
       <color rgb="FF9C5700"/>
       <name val="Aptos Display"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -553,17 +713,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -580,22 +741,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -928,15 +1087,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1293D70B-0512-624F-91B3-17CA08CDE41F}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="1" bestFit="1" customWidth="1"/>
@@ -975,6 +1134,9 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -986,6 +1148,9 @@
       <c r="D3" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -997,6 +1162,9 @@
       <c r="D4" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="E4" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>73</v>
       </c>
@@ -1011,6 +1179,9 @@
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1022,6 +1193,9 @@
       <c r="D6" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -1033,90 +1207,108 @@
       <c r="D7" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="E13" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -1128,6 +1320,9 @@
       <c r="D14" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="E14" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -1139,6 +1334,9 @@
       <c r="D15" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="E15" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -1150,6 +1348,9 @@
       <c r="D16" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="E16" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -1161,654 +1362,1010 @@
       <c r="D17" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="E17" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="E18" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="E19" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="E20" s="4" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6" t="s">
+      <c r="C23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="E23" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6" t="s">
+      <c r="C24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6" t="s">
+      <c r="E24" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6" t="s">
+      <c r="D25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="E25" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6" t="s">
+      <c r="D26" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5" t="s">
+      <c r="E26" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D27" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="E27" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7" t="s">
-        <v>101</v>
+      <c r="E28" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="C34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4" t="s">
+      <c r="C35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7" t="s">
-        <v>110</v>
+      <c r="E35" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="E43" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="4" t="s">
+      <c r="D47" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4" t="s">
+      <c r="E47" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D48" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7" t="s">
+      <c r="E48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>126</v>
+        <v>51</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>127</v>
+        <v>52</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>127</v>
+        <v>52</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54"/>
-      <c r="C54" t="s">
-        <v>132</v>
-      </c>
-      <c r="D54" t="s">
+        <v>124</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E54"/>
-      <c r="F54" t="s">
-        <v>133</v>
+      <c r="E54" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5" t="s">
-        <v>137</v>
+        <v>127</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D60" s="1" t="s">
+      <c r="C62" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="7" t="s">
+      <c r="E62" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
-        <v>67</v>
+        <v>138</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F63" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="C66" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+      <c r="D66" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D65" s="1" t="s">
+      <c r="C67" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>70</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B36522F-16CB-E64F-B8AC-661AE8C6BD81}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip: update theme tables (#844)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689B5B3E-4D82-9040-828A-7D880B6B3773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465A2C25-AD4B-854D-92E5-3BB0FA4D7011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="202">
   <si>
     <t>Layout Property</t>
   </si>
@@ -305,36 +306,24 @@
     <t>radius-start-start</t>
   </si>
   <si>
-    <t>We do not implement top-left, only the direction-aware start-start</t>
-  </si>
-  <si>
     <t>border-top-right-radius</t>
   </si>
   <si>
     <t>radius-start-end</t>
   </si>
   <si>
-    <t>We do not implement top-right, only the direction-aware start-end</t>
-  </si>
-  <si>
     <t>border-bottom-left-radius</t>
   </si>
   <si>
     <t>radius-end-start</t>
   </si>
   <si>
-    <t>We do not implement bottom-left, only the direction-aware end-start</t>
-  </si>
-  <si>
     <t>border-bottom-right-radius</t>
   </si>
   <si>
     <t>radius-end-end</t>
   </si>
   <si>
-    <t>We do not implement bottom-right, only the direction-aware end-end</t>
-  </si>
-  <si>
     <t>padding-horizontal</t>
   </si>
   <si>
@@ -477,13 +466,190 @@
   </si>
   <si>
     <t>white-space</t>
+  </si>
+  <si>
+    <t>maxWidth-content</t>
+  </si>
+  <si>
+    <t>We do not use these theme variables yet. Nonetheless, they may be used in the future</t>
+  </si>
+  <si>
+    <t>borderHorizontal</t>
+  </si>
+  <si>
+    <t>borderVertical</t>
+  </si>
+  <si>
+    <t>borderRadius</t>
+  </si>
+  <si>
+    <t>borderRadiusStartStart</t>
+  </si>
+  <si>
+    <t>borderRadiusStartEnd</t>
+  </si>
+  <si>
+    <t>borderRadiusEndStart</t>
+  </si>
+  <si>
+    <t>borderRadiusEndEnd</t>
+  </si>
+  <si>
+    <t>borderWidth</t>
+  </si>
+  <si>
+    <t>paddingHorizontal</t>
+  </si>
+  <si>
+    <t>paddingVertical</t>
+  </si>
+  <si>
+    <t>marginHorizontal</t>
+  </si>
+  <si>
+    <t>marginVertical</t>
+  </si>
+  <si>
+    <t>boxShadow</t>
+  </si>
+  <si>
+    <t>overflowX</t>
+  </si>
+  <si>
+    <t>overflowY</t>
+  </si>
+  <si>
+    <t>fontStyle</t>
+  </si>
+  <si>
+    <t>transformText</t>
+  </si>
+  <si>
+    <t>scroll-padding-block-Pages</t>
+  </si>
+  <si>
+    <t>scrollPaddingBlock-Pages</t>
+  </si>
+  <si>
+    <t>Special theme variable</t>
+  </si>
+  <si>
+    <t>New name</t>
+  </si>
+  <si>
+    <t>logo-AppHeader</t>
+  </si>
+  <si>
+    <t>align-content-AppHeader</t>
+  </si>
+  <si>
+    <t>justifyContent-AppHeader</t>
+  </si>
+  <si>
+    <t>thickness-outline</t>
+  </si>
+  <si>
+    <t>outlineWidth</t>
+  </si>
+  <si>
+    <t>color-outline</t>
+  </si>
+  <si>
+    <t>outlineColor</t>
+  </si>
+  <si>
+    <t>style-outline</t>
+  </si>
+  <si>
+    <t>outlineStyle</t>
+  </si>
+  <si>
+    <t>offset-outline</t>
+  </si>
+  <si>
+    <t>outlineOffset</t>
+  </si>
+  <si>
+    <t>textDecorationLine</t>
+  </si>
+  <si>
+    <t>textDecorationColor</t>
+  </si>
+  <si>
+    <t>textDecorationStyle</t>
+  </si>
+  <si>
+    <t>textDecorationThickness</t>
+  </si>
+  <si>
+    <t>text-decoration-line</t>
+  </si>
+  <si>
+    <t>text-decoration-color</t>
+  </si>
+  <si>
+    <t>text-decoration-style</t>
+  </si>
+  <si>
+    <t>text-decoration-thickness</t>
+  </si>
+  <si>
+    <t>textUnderlineOffset</t>
+  </si>
+  <si>
+    <t>text-underline-offset</t>
+  </si>
+  <si>
+    <t>outline-width</t>
+  </si>
+  <si>
+    <t>outline-color</t>
+  </si>
+  <si>
+    <t>line-decoration</t>
+  </si>
+  <si>
+    <t>color-decoration</t>
+  </si>
+  <si>
+    <t>style-decoration</t>
+  </si>
+  <si>
+    <t>thickness-decoration</t>
+  </si>
+  <si>
+    <t>offset-decoration</t>
+  </si>
+  <si>
+    <t>width-outline</t>
+  </si>
+  <si>
+    <t>outline-style</t>
+  </si>
+  <si>
+    <t>writing-mode</t>
+  </si>
+  <si>
+    <t>Review Text (put to layout context, along with direction)</t>
+  </si>
+  <si>
+    <t>align-items</t>
+  </si>
+  <si>
+    <t>alignItems</t>
+  </si>
+  <si>
+    <t>align-content</t>
+  </si>
+  <si>
+    <t>alignContent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -506,13 +672,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF9C0006"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -527,12 +686,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Display"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF9C0006"/>
       <name val="Aptos Display"/>
       <scheme val="major"/>
@@ -542,6 +695,13 @@
       <color rgb="FF9C5700"/>
       <name val="Aptos Display"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -553,17 +713,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -580,22 +741,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -928,15 +1087,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1293D70B-0512-624F-91B3-17CA08CDE41F}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="1" bestFit="1" customWidth="1"/>
@@ -975,6 +1134,9 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -986,6 +1148,9 @@
       <c r="D3" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -997,6 +1162,9 @@
       <c r="D4" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="E4" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>73</v>
       </c>
@@ -1011,6 +1179,9 @@
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1022,6 +1193,9 @@
       <c r="D6" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -1033,90 +1207,108 @@
       <c r="D7" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="E13" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -1128,6 +1320,9 @@
       <c r="D14" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="E14" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -1139,6 +1334,9 @@
       <c r="D15" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="E15" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -1150,6 +1348,9 @@
       <c r="D16" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="E16" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -1161,654 +1362,1010 @@
       <c r="D17" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="E17" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="E18" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="E19" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="E20" s="4" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6" t="s">
+      <c r="C23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="E23" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6" t="s">
+      <c r="C24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6" t="s">
+      <c r="E24" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6" t="s">
+      <c r="D25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="E25" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6" t="s">
+      <c r="D26" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5" t="s">
+      <c r="E26" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D27" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="E27" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7" t="s">
-        <v>101</v>
+      <c r="E28" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="C34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4" t="s">
+      <c r="C35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7" t="s">
-        <v>110</v>
+      <c r="E35" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="E43" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="4" t="s">
+      <c r="D47" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4" t="s">
+      <c r="E47" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D48" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7" t="s">
+      <c r="E48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>126</v>
+        <v>51</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>127</v>
+        <v>52</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>127</v>
+        <v>52</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54"/>
-      <c r="C54" t="s">
-        <v>132</v>
-      </c>
-      <c r="D54" t="s">
+        <v>124</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E54"/>
-      <c r="F54" t="s">
-        <v>133</v>
+      <c r="E54" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5" t="s">
-        <v>137</v>
+        <v>127</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D60" s="1" t="s">
+      <c r="C62" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="7" t="s">
+      <c r="E62" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
-        <v>67</v>
+        <v>138</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F63" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="C66" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+      <c r="D66" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D65" s="1" t="s">
+      <c r="C67" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>70</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B36522F-16CB-E64F-B8AC-661AE8C6BD81}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add new layout properties
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465A2C25-AD4B-854D-92E5-3BB0FA4D7011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1185CF63-1BDC-AC4C-9C64-6A634B1E8942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="199">
   <si>
     <t>Layout Property</t>
   </si>
@@ -627,22 +627,13 @@
     <t>outline-style</t>
   </si>
   <si>
-    <t>writing-mode</t>
-  </si>
-  <si>
-    <t>Review Text (put to layout context, along with direction)</t>
-  </si>
-  <si>
-    <t>align-items</t>
-  </si>
-  <si>
     <t>alignItems</t>
   </si>
   <si>
-    <t>align-content</t>
-  </si>
-  <si>
     <t>alignContent</t>
+  </si>
+  <si>
+    <t>outline-offset</t>
   </si>
 </sst>
 </file>
@@ -1089,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1293D70B-0512-624F-91B3-17CA08CDE41F}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:XFD78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2133,7 +2124,9 @@
         <v>127</v>
       </c>
       <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
+      <c r="E68" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2265,27 +2258,27 @@
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E78" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F77" s="1" t="s">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E79" s="1" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add new layout properties (#855)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465A2C25-AD4B-854D-92E5-3BB0FA4D7011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1185CF63-1BDC-AC4C-9C64-6A634B1E8942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="199">
   <si>
     <t>Layout Property</t>
   </si>
@@ -627,22 +627,13 @@
     <t>outline-style</t>
   </si>
   <si>
-    <t>writing-mode</t>
-  </si>
-  <si>
-    <t>Review Text (put to layout context, along with direction)</t>
-  </si>
-  <si>
-    <t>align-items</t>
-  </si>
-  <si>
     <t>alignItems</t>
   </si>
   <si>
-    <t>align-content</t>
-  </si>
-  <si>
     <t>alignContent</t>
+  </si>
+  <si>
+    <t>outline-offset</t>
   </si>
 </sst>
 </file>
@@ -1089,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1293D70B-0512-624F-91B3-17CA08CDE41F}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:XFD78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2133,7 +2124,9 @@
         <v>127</v>
       </c>
       <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
+      <c r="E68" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2265,27 +2258,27 @@
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E78" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F77" s="1" t="s">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E79" s="1" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: prepare for layout property renaming
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1185CF63-1BDC-AC4C-9C64-6A634B1E8942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E9618E-365D-0045-8EF5-E4BA946CE1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Layout and Theme vars" sheetId="3" r:id="rId1"/>
+    <sheet name="Changelog" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,16 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="199">
-  <si>
-    <t>Layout Property</t>
-  </si>
-  <si>
-    <t>CSS Property</t>
-  </si>
-  <si>
-    <t>Theme Variable</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="190">
   <si>
     <t>width</t>
   </si>
@@ -105,12 +96,6 @@
     <t>borderThickness</t>
   </si>
   <si>
-    <t>New Layout Name</t>
-  </si>
-  <si>
-    <t>New Theme Variable Name</t>
-  </si>
-  <si>
     <t>radius</t>
   </si>
   <si>
@@ -234,12 +219,6 @@
     <t>textAlignLast</t>
   </si>
   <si>
-    <t>wrapContent</t>
-  </si>
-  <si>
-    <t>canShrink</t>
-  </si>
-  <si>
     <t>cursor</t>
   </si>
   <si>
@@ -300,21 +279,12 @@
     <t>border-radius</t>
   </si>
   <si>
-    <t>border-top-left-radius</t>
-  </si>
-  <si>
     <t>radius-start-start</t>
   </si>
   <si>
-    <t>border-top-right-radius</t>
-  </si>
-  <si>
     <t>radius-start-end</t>
   </si>
   <si>
-    <t>border-bottom-left-radius</t>
-  </si>
-  <si>
     <t>radius-end-start</t>
   </si>
   <si>
@@ -330,12 +300,6 @@
     <t>padding-vertical</t>
   </si>
   <si>
-    <t>Sets the padding-top and padding-bottom styles</t>
-  </si>
-  <si>
-    <t>Sets the padding-left and padding-right styles</t>
-  </si>
-  <si>
     <t>padding-top</t>
   </si>
   <si>
@@ -354,12 +318,6 @@
     <t>margin-vertical</t>
   </si>
   <si>
-    <t>Sets the margin-left and margin-right styles</t>
-  </si>
-  <si>
-    <t>Sets the margin-top and margin-bottom styles</t>
-  </si>
-  <si>
     <t>margin-top</t>
   </si>
   <si>
@@ -378,15 +336,9 @@
     <t>color-bg</t>
   </si>
   <si>
-    <t>Do we want to use it as an alias for "color-bg"?</t>
-  </si>
-  <si>
     <t>box-shadow</t>
   </si>
   <si>
-    <t>If we had such a theme variable, we used "direction"</t>
-  </si>
-  <si>
     <t>overflow-x</t>
   </si>
   <si>
@@ -453,27 +405,12 @@
     <t>text-wrap</t>
   </si>
   <si>
-    <t>flex-wrap</t>
-  </si>
-  <si>
-    <t>We use "wrapContent" as a boolean property resulting "flex-wrap: wrap" for true and "flex-wrap: nowrap" for false</t>
-  </si>
-  <si>
-    <t>flex-shrink</t>
-  </si>
-  <si>
-    <t>We use "canShrink" as a boolean property resulting "flex-shrink: 1" for true and "flex-shrink: 0" for false</t>
-  </si>
-  <si>
     <t>white-space</t>
   </si>
   <si>
     <t>maxWidth-content</t>
   </si>
   <si>
-    <t>We do not use these theme variables yet. Nonetheless, they may be used in the future</t>
-  </si>
-  <si>
     <t>borderHorizontal</t>
   </si>
   <si>
@@ -525,30 +462,6 @@
     <t>transformText</t>
   </si>
   <si>
-    <t>scroll-padding-block-Pages</t>
-  </si>
-  <si>
-    <t>scrollPaddingBlock-Pages</t>
-  </si>
-  <si>
-    <t>Special theme variable</t>
-  </si>
-  <si>
-    <t>New name</t>
-  </si>
-  <si>
-    <t>logo-AppHeader</t>
-  </si>
-  <si>
-    <t>align-content-AppHeader</t>
-  </si>
-  <si>
-    <t>justifyContent-AppHeader</t>
-  </si>
-  <si>
-    <t>thickness-outline</t>
-  </si>
-  <si>
     <t>outlineWidth</t>
   </si>
   <si>
@@ -627,20 +540,80 @@
     <t>outline-style</t>
   </si>
   <si>
-    <t>alignItems</t>
-  </si>
-  <si>
-    <t>alignContent</t>
-  </si>
-  <si>
     <t>outline-offset</t>
+  </si>
+  <si>
+    <t>Related CSS Property</t>
+  </si>
+  <si>
+    <t>Theme Var Prefix</t>
+  </si>
+  <si>
+    <t>Layout Property Name</t>
+  </si>
+  <si>
+    <t>New Property Name</t>
+  </si>
+  <si>
+    <t>New Theme Var Prefix</t>
+  </si>
+  <si>
+    <t>Maps to the border-top and border-bottom CSS properties</t>
+  </si>
+  <si>
+    <t>Maps to the border-left and border-right CSS properties</t>
+  </si>
+  <si>
+    <t>max-…-width</t>
+  </si>
+  <si>
+    <t>border-horizontal</t>
+  </si>
+  <si>
+    <t>border-vertical</t>
+  </si>
+  <si>
+    <t>border-radius-start-start</t>
+  </si>
+  <si>
+    <t>borde-radius-start-end</t>
+  </si>
+  <si>
+    <t>border-radius-end-start</t>
+  </si>
+  <si>
+    <t>Sets the padding-left and padding-right CSS properties</t>
+  </si>
+  <si>
+    <t>Sets the padding-top and padding-bottom CSS properties</t>
+  </si>
+  <si>
+    <t>Sets the margin-left and margin-right CSS properties</t>
+  </si>
+  <si>
+    <t>Sets the margin-top and margin-bottom CSS properties</t>
+  </si>
+  <si>
+    <t>scroll-horizontal</t>
+  </si>
+  <si>
+    <t>scroll-vertical</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Introduce borderHorizontal</t>
+  </si>
+  <si>
+    <t>Introduce borderVertical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -663,23 +636,10 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF9C5700"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Display"/>
-      <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
@@ -689,13 +649,19 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -704,18 +670,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -728,24 +688,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1077,17 +1034,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1293D70B-0512-624F-91B3-17CA08CDE41F}">
-  <dimension ref="A1:F79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:XFD78"/>
+    <sheetView topLeftCell="A47" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" style="1" bestFit="1" customWidth="1"/>
@@ -1097,1268 +1054,1338 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>22</v>
+        <v>171</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>168</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>169</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>23</v>
+        <v>172</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>40</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>4</v>
+        <v>98</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>70</v>
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>71</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>7</v>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>124</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>8</v>
+        <v>176</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>144</v>
+        <v>72</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>144</v>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>144</v>
+        <v>76</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>144</v>
+        <v>78</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>144</v>
+        <v>69</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>125</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>177</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>76</v>
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>77</v>
+      <c r="A15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>78</v>
+      <c r="A16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>18</v>
+        <v>42</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>19</v>
+        <v>106</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>20</v>
+        <v>107</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>152</v>
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>152</v>
+        <v>108</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>70</v>
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>145</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
-        <v>146</v>
+      <c r="A22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>146</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>147</v>
+        <v>91</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>148</v>
+        <v>185</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B25" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="C25" s="1" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>149</v>
+        <v>85</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>150</v>
+        <v>63</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>94</v>
+      <c r="A27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>151</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>30</v>
+        <v>114</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>153</v>
+        <v>56</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>98</v>
+        <v>118</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>96</v>
+      <c r="B30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>33</v>
+        <v>95</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>34</v>
+        <v>96</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>35</v>
+        <v>94</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>36</v>
+        <v>93</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>155</v>
+        <v>2</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>155</v>
+        <v>175</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>105</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>156</v>
+        <v>4</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>106</v>
+        <v>67</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>1</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>40</v>
+        <v>64</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>108</v>
+      <c r="A39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>143</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>109</v>
+        <v>159</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>42</v>
+        <v>142</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>147</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>110</v>
+        <v>167</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>43</v>
+        <v>146</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>44</v>
+        <v>145</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>111</v>
+        <v>166</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>44</v>
+        <v>144</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>141</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>113</v>
+        <v>165</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>46</v>
+      <c r="A44" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>157</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>115</v>
+        <v>89</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>158</v>
+        <v>31</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>118</v>
+        <v>90</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>159</v>
+        <v>29</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>119</v>
+        <v>88</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>28</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>121</v>
+        <v>87</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>19</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>51</v>
+        <v>19</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>52</v>
+        <v>180</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>52</v>
+        <v>82</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>23</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>53</v>
+        <v>84</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>123</v>
+        <v>178</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>21</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>55</v>
+        <v>81</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>70</v>
+      <c r="A54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>126</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>57</v>
+        <v>41</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="B57" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="C57" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E57" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>133</v>
+        <v>111</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>61</v>
+        <v>149</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>61</v>
+        <v>161</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>62</v>
+        <v>148</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>62</v>
+        <v>160</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>63</v>
+        <v>150</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>63</v>
+        <v>162</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>64</v>
+        <v>151</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>64</v>
+        <v>163</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3" t="s">
-        <v>139</v>
+      <c r="A63" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3" t="s">
-        <v>141</v>
+      <c r="A64" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>67</v>
+        <v>121</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>68</v>
+      <c r="A66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F68" s="5"/>
+      <c r="A68" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="F69" s="5"/>
+      <c r="A69" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5" t="s">
+      <c r="A70" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="F71" s="5"/>
+      <c r="A71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="F72" s="5"/>
+      <c r="A72" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="F73" s="5"/>
+      <c r="A73" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F74" s="5"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="F75" s="5"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F76" s="5"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="F77" s="5"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E78" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E79" s="1" t="s">
-        <v>197</v>
+      <c r="A74" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F79">
+    <sortCondition ref="A2:A79"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B36522F-16CB-E64F-B8AC-661AE8C6BD81}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" t="s">
-        <v>176</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: prepare for layout property renaming (#858)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1185CF63-1BDC-AC4C-9C64-6A634B1E8942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E9618E-365D-0045-8EF5-E4BA946CE1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Layout and Theme vars" sheetId="3" r:id="rId1"/>
+    <sheet name="Changelog" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,16 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="199">
-  <si>
-    <t>Layout Property</t>
-  </si>
-  <si>
-    <t>CSS Property</t>
-  </si>
-  <si>
-    <t>Theme Variable</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="190">
   <si>
     <t>width</t>
   </si>
@@ -105,12 +96,6 @@
     <t>borderThickness</t>
   </si>
   <si>
-    <t>New Layout Name</t>
-  </si>
-  <si>
-    <t>New Theme Variable Name</t>
-  </si>
-  <si>
     <t>radius</t>
   </si>
   <si>
@@ -234,12 +219,6 @@
     <t>textAlignLast</t>
   </si>
   <si>
-    <t>wrapContent</t>
-  </si>
-  <si>
-    <t>canShrink</t>
-  </si>
-  <si>
     <t>cursor</t>
   </si>
   <si>
@@ -300,21 +279,12 @@
     <t>border-radius</t>
   </si>
   <si>
-    <t>border-top-left-radius</t>
-  </si>
-  <si>
     <t>radius-start-start</t>
   </si>
   <si>
-    <t>border-top-right-radius</t>
-  </si>
-  <si>
     <t>radius-start-end</t>
   </si>
   <si>
-    <t>border-bottom-left-radius</t>
-  </si>
-  <si>
     <t>radius-end-start</t>
   </si>
   <si>
@@ -330,12 +300,6 @@
     <t>padding-vertical</t>
   </si>
   <si>
-    <t>Sets the padding-top and padding-bottom styles</t>
-  </si>
-  <si>
-    <t>Sets the padding-left and padding-right styles</t>
-  </si>
-  <si>
     <t>padding-top</t>
   </si>
   <si>
@@ -354,12 +318,6 @@
     <t>margin-vertical</t>
   </si>
   <si>
-    <t>Sets the margin-left and margin-right styles</t>
-  </si>
-  <si>
-    <t>Sets the margin-top and margin-bottom styles</t>
-  </si>
-  <si>
     <t>margin-top</t>
   </si>
   <si>
@@ -378,15 +336,9 @@
     <t>color-bg</t>
   </si>
   <si>
-    <t>Do we want to use it as an alias for "color-bg"?</t>
-  </si>
-  <si>
     <t>box-shadow</t>
   </si>
   <si>
-    <t>If we had such a theme variable, we used "direction"</t>
-  </si>
-  <si>
     <t>overflow-x</t>
   </si>
   <si>
@@ -453,27 +405,12 @@
     <t>text-wrap</t>
   </si>
   <si>
-    <t>flex-wrap</t>
-  </si>
-  <si>
-    <t>We use "wrapContent" as a boolean property resulting "flex-wrap: wrap" for true and "flex-wrap: nowrap" for false</t>
-  </si>
-  <si>
-    <t>flex-shrink</t>
-  </si>
-  <si>
-    <t>We use "canShrink" as a boolean property resulting "flex-shrink: 1" for true and "flex-shrink: 0" for false</t>
-  </si>
-  <si>
     <t>white-space</t>
   </si>
   <si>
     <t>maxWidth-content</t>
   </si>
   <si>
-    <t>We do not use these theme variables yet. Nonetheless, they may be used in the future</t>
-  </si>
-  <si>
     <t>borderHorizontal</t>
   </si>
   <si>
@@ -525,30 +462,6 @@
     <t>transformText</t>
   </si>
   <si>
-    <t>scroll-padding-block-Pages</t>
-  </si>
-  <si>
-    <t>scrollPaddingBlock-Pages</t>
-  </si>
-  <si>
-    <t>Special theme variable</t>
-  </si>
-  <si>
-    <t>New name</t>
-  </si>
-  <si>
-    <t>logo-AppHeader</t>
-  </si>
-  <si>
-    <t>align-content-AppHeader</t>
-  </si>
-  <si>
-    <t>justifyContent-AppHeader</t>
-  </si>
-  <si>
-    <t>thickness-outline</t>
-  </si>
-  <si>
     <t>outlineWidth</t>
   </si>
   <si>
@@ -627,20 +540,80 @@
     <t>outline-style</t>
   </si>
   <si>
-    <t>alignItems</t>
-  </si>
-  <si>
-    <t>alignContent</t>
-  </si>
-  <si>
     <t>outline-offset</t>
+  </si>
+  <si>
+    <t>Related CSS Property</t>
+  </si>
+  <si>
+    <t>Theme Var Prefix</t>
+  </si>
+  <si>
+    <t>Layout Property Name</t>
+  </si>
+  <si>
+    <t>New Property Name</t>
+  </si>
+  <si>
+    <t>New Theme Var Prefix</t>
+  </si>
+  <si>
+    <t>Maps to the border-top and border-bottom CSS properties</t>
+  </si>
+  <si>
+    <t>Maps to the border-left and border-right CSS properties</t>
+  </si>
+  <si>
+    <t>max-…-width</t>
+  </si>
+  <si>
+    <t>border-horizontal</t>
+  </si>
+  <si>
+    <t>border-vertical</t>
+  </si>
+  <si>
+    <t>border-radius-start-start</t>
+  </si>
+  <si>
+    <t>borde-radius-start-end</t>
+  </si>
+  <si>
+    <t>border-radius-end-start</t>
+  </si>
+  <si>
+    <t>Sets the padding-left and padding-right CSS properties</t>
+  </si>
+  <si>
+    <t>Sets the padding-top and padding-bottom CSS properties</t>
+  </si>
+  <si>
+    <t>Sets the margin-left and margin-right CSS properties</t>
+  </si>
+  <si>
+    <t>Sets the margin-top and margin-bottom CSS properties</t>
+  </si>
+  <si>
+    <t>scroll-horizontal</t>
+  </si>
+  <si>
+    <t>scroll-vertical</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Introduce borderHorizontal</t>
+  </si>
+  <si>
+    <t>Introduce borderVertical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -663,23 +636,10 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF9C5700"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Display"/>
-      <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
@@ -689,13 +649,19 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -704,18 +670,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -728,24 +688,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1077,17 +1034,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1293D70B-0512-624F-91B3-17CA08CDE41F}">
-  <dimension ref="A1:F79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:XFD78"/>
+    <sheetView topLeftCell="A47" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" style="1" bestFit="1" customWidth="1"/>
@@ -1097,1268 +1054,1338 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>22</v>
+        <v>171</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>168</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>169</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>23</v>
+        <v>172</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>40</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>4</v>
+        <v>98</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>70</v>
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>71</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>7</v>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>124</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>8</v>
+        <v>176</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>144</v>
+        <v>72</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>144</v>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>144</v>
+        <v>76</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>144</v>
+        <v>78</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>144</v>
+        <v>69</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>125</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>177</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>76</v>
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>77</v>
+      <c r="A15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>78</v>
+      <c r="A16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>18</v>
+        <v>42</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>19</v>
+        <v>106</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>20</v>
+        <v>107</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>152</v>
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>152</v>
+        <v>108</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>70</v>
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>145</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
-        <v>146</v>
+      <c r="A22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>146</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>147</v>
+        <v>91</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>148</v>
+        <v>185</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B25" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="C25" s="1" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>149</v>
+        <v>85</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>150</v>
+        <v>63</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>94</v>
+      <c r="A27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>151</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>30</v>
+        <v>114</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>153</v>
+        <v>56</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>98</v>
+        <v>118</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>96</v>
+      <c r="B30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>33</v>
+        <v>95</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>34</v>
+        <v>96</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>35</v>
+        <v>94</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>36</v>
+        <v>93</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>155</v>
+        <v>2</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>155</v>
+        <v>175</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>105</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>156</v>
+        <v>4</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>106</v>
+        <v>67</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>1</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>40</v>
+        <v>64</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>108</v>
+      <c r="A39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>143</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>109</v>
+        <v>159</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>42</v>
+        <v>142</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>147</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>110</v>
+        <v>167</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>43</v>
+        <v>146</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>44</v>
+        <v>145</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>111</v>
+        <v>166</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>44</v>
+        <v>144</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>141</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>113</v>
+        <v>165</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>46</v>
+      <c r="A44" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>157</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>115</v>
+        <v>89</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>158</v>
+        <v>31</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>118</v>
+        <v>90</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>159</v>
+        <v>29</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>119</v>
+        <v>88</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>28</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>121</v>
+        <v>87</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>19</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>51</v>
+        <v>19</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>52</v>
+        <v>180</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>52</v>
+        <v>82</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>23</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>53</v>
+        <v>84</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>123</v>
+        <v>178</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>21</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>55</v>
+        <v>81</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>70</v>
+      <c r="A54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>126</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>57</v>
+        <v>41</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="B57" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="C57" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E57" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>133</v>
+        <v>111</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>61</v>
+        <v>149</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>61</v>
+        <v>161</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>62</v>
+        <v>148</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>62</v>
+        <v>160</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>63</v>
+        <v>150</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>63</v>
+        <v>162</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>64</v>
+        <v>151</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>64</v>
+        <v>163</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3" t="s">
-        <v>139</v>
+      <c r="A63" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3" t="s">
-        <v>141</v>
+      <c r="A64" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>67</v>
+        <v>121</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>68</v>
+      <c r="A66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F68" s="5"/>
+      <c r="A68" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="F69" s="5"/>
+      <c r="A69" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5" t="s">
+      <c r="A70" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="F71" s="5"/>
+      <c r="A71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="F72" s="5"/>
+      <c r="A72" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="F73" s="5"/>
+      <c r="A73" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F74" s="5"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="F75" s="5"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F76" s="5"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="F77" s="5"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E78" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E79" s="1" t="s">
-        <v>197</v>
+      <c r="A74" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F79">
+    <sortCondition ref="A2:A79"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B36522F-16CB-E64F-B8AC-661AE8C6BD81}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" t="s">
-        <v>176</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: rename "italic" to "fontStyle"
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E9618E-365D-0045-8EF5-E4BA946CE1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BB6FBF-F50D-9343-AFB0-2ABBBECC9C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="191">
   <si>
     <t>width</t>
   </si>
@@ -607,6 +607,9 @@
   </si>
   <si>
     <t>Introduce borderVertical</t>
+  </si>
+  <si>
+    <t>italic --&gt; fontStyle</t>
   </si>
 </sst>
 </file>
@@ -2362,10 +2365,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2388,6 +2391,11 @@
         <v>189</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>190</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: rename "italic" to "fontStyle" (#859)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E9618E-365D-0045-8EF5-E4BA946CE1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BB6FBF-F50D-9343-AFB0-2ABBBECC9C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="191">
   <si>
     <t>width</t>
   </si>
@@ -607,6 +607,9 @@
   </si>
   <si>
     <t>Introduce borderVertical</t>
+  </si>
+  <si>
+    <t>italic --&gt; fontStyle</t>
   </si>
 </sst>
 </file>
@@ -2362,10 +2365,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2388,6 +2391,11 @@
         <v>189</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>190</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: change "borderThickness" to "borderWidth"
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BB6FBF-F50D-9343-AFB0-2ABBBECC9C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4E32DE-393D-964B-A020-1FB1623AB32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="193">
   <si>
     <t>width</t>
   </si>
@@ -610,6 +610,12 @@
   </si>
   <si>
     <t>italic --&gt; fontStyle</t>
+  </si>
+  <si>
+    <t>shadow --&gt; boxShadow</t>
+  </si>
+  <si>
+    <t>borderThickness --&gt; borderWidth</t>
   </si>
 </sst>
 </file>
@@ -1040,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1164,7 +1170,7 @@
       <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>124</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1235,7 +1241,7 @@
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>131</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1269,7 +1275,7 @@
       <c r="A13" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1502,7 +1508,7 @@
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>139</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -2001,7 +2007,7 @@
       <c r="A55" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -2365,15 +2371,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -2396,6 +2402,16 @@
         <v>190</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>192</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: change "borderThickness" to "borderWidth" (#862)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BB6FBF-F50D-9343-AFB0-2ABBBECC9C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4E32DE-393D-964B-A020-1FB1623AB32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="193">
   <si>
     <t>width</t>
   </si>
@@ -610,6 +610,12 @@
   </si>
   <si>
     <t>italic --&gt; fontStyle</t>
+  </si>
+  <si>
+    <t>shadow --&gt; boxShadow</t>
+  </si>
+  <si>
+    <t>borderThickness --&gt; borderWidth</t>
   </si>
 </sst>
 </file>
@@ -1040,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1164,7 +1170,7 @@
       <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>124</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1235,7 +1241,7 @@
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>131</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1269,7 +1275,7 @@
       <c r="A13" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1502,7 +1508,7 @@
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>139</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -2001,7 +2007,7 @@
       <c r="A55" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -2365,15 +2371,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -2396,6 +2402,16 @@
         <v>190</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>192</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: layout props: horizontalMargin --> marginHorizontal, verticalMargin --> marginVertical
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4E32DE-393D-964B-A020-1FB1623AB32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E792B3E2-741F-154C-B3C7-C11FBB26A115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="195">
   <si>
     <t>width</t>
   </si>
@@ -616,6 +616,12 @@
   </si>
   <si>
     <t>borderThickness --&gt; borderWidth</t>
+  </si>
+  <si>
+    <t>horizontalMargin --&gt; marginHorizontal</t>
+  </si>
+  <si>
+    <t>verticalMargin --&gt; marginVertical</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1053,7 @@
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1448,7 +1454,7 @@
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>134</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -2234,7 +2240,7 @@
       <c r="A68" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="4" t="s">
         <v>135</v>
       </c>
       <c r="C68" s="1" t="s">
@@ -2371,15 +2377,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -2412,6 +2418,16 @@
         <v>192</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: layout props: horizontalMargin --> marginHorizontal, verticalMargin --> marginVertical (#882)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4E32DE-393D-964B-A020-1FB1623AB32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E792B3E2-741F-154C-B3C7-C11FBB26A115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="195">
   <si>
     <t>width</t>
   </si>
@@ -616,6 +616,12 @@
   </si>
   <si>
     <t>borderThickness --&gt; borderWidth</t>
+  </si>
+  <si>
+    <t>horizontalMargin --&gt; marginHorizontal</t>
+  </si>
+  <si>
+    <t>verticalMargin --&gt; marginVertical</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1053,7 @@
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1448,7 +1454,7 @@
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>134</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -2234,7 +2240,7 @@
       <c r="A68" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="4" t="s">
         <v>135</v>
       </c>
       <c r="C68" s="1" t="s">
@@ -2371,15 +2377,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -2412,6 +2418,16 @@
         <v>192</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: rename props: horizontalPadding --> paddingHorizontal, verticalPadding --> paddingVertical (#884)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E792B3E2-741F-154C-B3C7-C11FBB26A115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9817FE-D8B1-D64B-93EC-700EA976DFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout and Theme vars" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="197">
   <si>
     <t>width</t>
   </si>
@@ -622,6 +622,12 @@
   </si>
   <si>
     <t>verticalMargin --&gt; marginVertical</t>
+  </si>
+  <si>
+    <t>horizontalPadding --&gt; paddingHorizontal</t>
+  </si>
+  <si>
+    <t>verticalPadding --&gt; paddingVertical</t>
   </si>
 </sst>
 </file>
@@ -1052,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1474,7 +1480,7 @@
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1494,7 +1500,7 @@
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>132</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -2260,7 +2266,7 @@
       <c r="A69" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="4" t="s">
         <v>138</v>
       </c>
       <c r="C69" s="1" t="s">
@@ -2280,7 +2286,7 @@
       <c r="A70" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="4" t="s">
         <v>133</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -2377,10 +2383,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2428,6 +2434,16 @@
         <v>194</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>196</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wip: zIndex, whiteSpace, userSelect, textWrap, textUnderlineOffset
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9817FE-D8B1-D64B-93EC-700EA976DFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAA71E9-5D12-3F46-A300-3DF5233C84ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -1059,7 +1059,7 @@
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2235,7 +2235,7 @@
       <c r="D67" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F67" s="1" t="s">
@@ -2315,7 +2315,7 @@
       <c r="D71" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E71" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2349,7 +2349,7 @@
       <c r="D73" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E73" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F73" s="1" t="s">

</xml_diff>

<commit_message>
wip: textDecoration, -Style, -Line, -Color
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF46D77A-9611-2D45-87A9-C2B1A75AF719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE499E60-6232-3D41-8461-8FBF7E7D6827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout and Theme vars" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="206">
   <si>
     <t>width</t>
   </si>
@@ -640,6 +640,21 @@
   </si>
   <si>
     <t>"transform-" --&gt; textTransform</t>
+  </si>
+  <si>
+    <t>thickness-decoration --&gt; textDecorationThickness</t>
+  </si>
+  <si>
+    <t>style-decoration --&gt; textDecorationStyle</t>
+  </si>
+  <si>
+    <t>line-decoration --&gt; textDecorationLine</t>
+  </si>
+  <si>
+    <t>color-decoration --&gt; textDecorationColor</t>
+  </si>
+  <si>
+    <t>text-decoration --&gt; textDecoration</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2091,7 +2106,7 @@
       <c r="D58" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2108,7 +2123,7 @@
       <c r="D59" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="4" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2125,7 +2140,7 @@
       <c r="D60" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="4" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2142,7 +2157,7 @@
       <c r="D61" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="4" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2159,7 +2174,7 @@
       <c r="D62" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="4" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2176,7 +2191,7 @@
       <c r="D63" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F63" s="1" t="s">
@@ -2398,15 +2413,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -2479,6 +2494,31 @@
         <v>200</v>
       </c>
     </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: rename theme variables (batch 1) (#885)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9817FE-D8B1-D64B-93EC-700EA976DFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE499E60-6232-3D41-8461-8FBF7E7D6827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="206">
   <si>
     <t>width</t>
   </si>
@@ -459,9 +459,6 @@
     <t>fontStyle</t>
   </si>
   <si>
-    <t>transformText</t>
-  </si>
-  <si>
     <t>outlineWidth</t>
   </si>
   <si>
@@ -628,6 +625,36 @@
   </si>
   <si>
     <t>verticalPadding --&gt; paddingVertical</t>
+  </si>
+  <si>
+    <t>(existing theme vars: offset-decoration)</t>
+  </si>
+  <si>
+    <t>offset-decoration --&gt; textUnderlineOffset</t>
+  </si>
+  <si>
+    <t>text-transform --&gt; textTransform</t>
+  </si>
+  <si>
+    <t>transform-text --&gt; textTransform</t>
+  </si>
+  <si>
+    <t>"transform-" --&gt; textTransform</t>
+  </si>
+  <si>
+    <t>thickness-decoration --&gt; textDecorationThickness</t>
+  </si>
+  <si>
+    <t>style-decoration --&gt; textDecorationStyle</t>
+  </si>
+  <si>
+    <t>line-decoration --&gt; textDecorationLine</t>
+  </si>
+  <si>
+    <t>color-decoration --&gt; textDecorationColor</t>
+  </si>
+  <si>
+    <t>text-decoration --&gt; textDecoration</t>
   </si>
 </sst>
 </file>
@@ -1058,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1075,19 +1102,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>24</v>
@@ -1189,13 +1216,13 @@
         <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>124</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1294,13 +1321,13 @@
         <v>63</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>125</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1473,7 +1500,7 @@
         <v>134</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1487,7 +1514,7 @@
         <v>100</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>137</v>
@@ -1513,7 +1540,7 @@
         <v>132</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1700,7 +1727,7 @@
         <v>65</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>123</v>
@@ -1762,70 +1789,70 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1938,7 +1965,7 @@
         <v>129</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>82</v>
@@ -1972,7 +1999,7 @@
         <v>127</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>80</v>
@@ -1989,7 +2016,7 @@
         <v>128</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>81</v>
@@ -2079,76 +2106,76 @@
       <c r="D58" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>149</v>
+        <v>160</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>148</v>
+        <v>159</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>150</v>
+        <v>161</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>151</v>
+        <v>162</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2164,8 +2191,8 @@
       <c r="D63" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>140</v>
+      <c r="E63" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>117</v>
@@ -2173,19 +2200,22 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="D64" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>156</v>
+        <v>163</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2201,7 +2231,7 @@
       <c r="D65" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2235,7 +2265,7 @@
       <c r="D67" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F67" s="1" t="s">
@@ -2259,7 +2289,7 @@
         <v>135</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2273,7 +2303,7 @@
         <v>101</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>138</v>
@@ -2299,7 +2329,7 @@
         <v>133</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2315,7 +2345,7 @@
       <c r="D71" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E71" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2349,7 +2379,7 @@
       <c r="D73" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E73" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F73" s="1" t="s">
@@ -2383,65 +2413,110 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>196</v>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip: shadow --> boxShadow
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE499E60-6232-3D41-8461-8FBF7E7D6827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE96999-893E-4649-9031-0801F6031C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="207">
   <si>
     <t>width</t>
   </si>
@@ -597,9 +597,6 @@
     <t>scroll-vertical</t>
   </si>
   <si>
-    <t>Changes</t>
-  </si>
-  <si>
     <t>Introduce borderHorizontal</t>
   </si>
   <si>
@@ -655,6 +652,12 @@
   </si>
   <si>
     <t>text-decoration --&gt; textDecoration</t>
+  </si>
+  <si>
+    <t>Changes (layout properties)</t>
+  </si>
+  <si>
+    <t>Changes (theme variables)</t>
   </si>
 </sst>
 </file>
@@ -1085,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2043,67 +2046,67 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="4" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="4" t="s">
         <v>111</v>
       </c>
       <c r="E58" s="4" t="s">
@@ -2111,16 +2114,16 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" s="4" t="s">
         <v>160</v>
       </c>
       <c r="E59" s="4" t="s">
@@ -2128,16 +2131,16 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="4" t="s">
         <v>159</v>
       </c>
       <c r="E60" s="4" t="s">
@@ -2145,16 +2148,16 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="4" t="s">
         <v>161</v>
       </c>
       <c r="E61" s="4" t="s">
@@ -2162,16 +2165,16 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" s="4" t="s">
         <v>162</v>
       </c>
       <c r="E62" s="4" t="s">
@@ -2179,16 +2182,16 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="4" t="s">
         <v>116</v>
       </c>
       <c r="E63" s="4" t="s">
@@ -2199,36 +2202,36 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" s="4" t="s">
         <v>163</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>155</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="4" t="s">
         <v>121</v>
       </c>
       <c r="E65" s="4" t="s">
@@ -2253,16 +2256,16 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E67" s="4" t="s">
@@ -2333,16 +2336,16 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E71" s="4" t="s">
@@ -2367,16 +2370,16 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E73" s="4" t="s">
@@ -2413,10 +2416,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2426,97 +2429,107 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>197</v>
+      <c r="A11" s="2" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>203</v>
+      <c r="A17" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>205</v>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: rename theme variables (batch 2) (#886)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE499E60-6232-3D41-8461-8FBF7E7D6827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE96999-893E-4649-9031-0801F6031C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="207">
   <si>
     <t>width</t>
   </si>
@@ -597,9 +597,6 @@
     <t>scroll-vertical</t>
   </si>
   <si>
-    <t>Changes</t>
-  </si>
-  <si>
     <t>Introduce borderHorizontal</t>
   </si>
   <si>
@@ -655,6 +652,12 @@
   </si>
   <si>
     <t>text-decoration --&gt; textDecoration</t>
+  </si>
+  <si>
+    <t>Changes (layout properties)</t>
+  </si>
+  <si>
+    <t>Changes (theme variables)</t>
   </si>
 </sst>
 </file>
@@ -1085,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2043,67 +2046,67 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="4" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="4" t="s">
         <v>111</v>
       </c>
       <c r="E58" s="4" t="s">
@@ -2111,16 +2114,16 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" s="4" t="s">
         <v>160</v>
       </c>
       <c r="E59" s="4" t="s">
@@ -2128,16 +2131,16 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="4" t="s">
         <v>159</v>
       </c>
       <c r="E60" s="4" t="s">
@@ -2145,16 +2148,16 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="4" t="s">
         <v>161</v>
       </c>
       <c r="E61" s="4" t="s">
@@ -2162,16 +2165,16 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" s="4" t="s">
         <v>162</v>
       </c>
       <c r="E62" s="4" t="s">
@@ -2179,16 +2182,16 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="4" t="s">
         <v>116</v>
       </c>
       <c r="E63" s="4" t="s">
@@ -2199,36 +2202,36 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" s="4" t="s">
         <v>163</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>155</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="4" t="s">
         <v>121</v>
       </c>
       <c r="E65" s="4" t="s">
@@ -2253,16 +2256,16 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E67" s="4" t="s">
@@ -2333,16 +2336,16 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E71" s="4" t="s">
@@ -2367,16 +2370,16 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E73" s="4" t="s">
@@ -2413,10 +2416,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2426,97 +2429,107 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>197</v>
+      <c r="A11" s="2" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>203</v>
+      <c r="A17" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>205</v>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip: margin and padding
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE96999-893E-4649-9031-0801F6031C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A10601-7F3D-B947-890C-6141BBA84E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout and Theme vars" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="225">
   <si>
     <t>width</t>
   </si>
@@ -531,9 +531,6 @@
     <t>offset-decoration</t>
   </si>
   <si>
-    <t>width-outline</t>
-  </si>
-  <si>
     <t>outline-style</t>
   </si>
   <si>
@@ -658,6 +655,63 @@
   </si>
   <si>
     <t>Changes (theme variables)</t>
+  </si>
+  <si>
+    <t>color-outline --&gt; outlineColor</t>
+  </si>
+  <si>
+    <t>offset-outline --&gt; outlineOffset</t>
+  </si>
+  <si>
+    <t>style-outline --&gt; outlineStyle</t>
+  </si>
+  <si>
+    <t>thickness-outline</t>
+  </si>
+  <si>
+    <t>thickness-outline --&gt; outlineWidth</t>
+  </si>
+  <si>
+    <t>letter-spacing --&gt; letterSpacing</t>
+  </si>
+  <si>
+    <t>line-height --&gt; lineHeight</t>
+  </si>
+  <si>
+    <t>font-family --&gt; fontFamily</t>
+  </si>
+  <si>
+    <t>font-size --&gt; fontSize</t>
+  </si>
+  <si>
+    <t>font-style --&gt; fontStyle</t>
+  </si>
+  <si>
+    <t>margin-horizontal --&gt; marginHorizontal</t>
+  </si>
+  <si>
+    <t>margin-vertical --&gt; marginVertical</t>
+  </si>
+  <si>
+    <t>scroll-horizontal --&gt; overflowX</t>
+  </si>
+  <si>
+    <t>scroll-vertical --&gt; overflowY</t>
+  </si>
+  <si>
+    <t>padding-horizontal --&gt; paddingHorizontal</t>
+  </si>
+  <si>
+    <t>padding-vertical --&gt; paddingVertical</t>
+  </si>
+  <si>
+    <t>padding-bottom --&gt; paddingBottom</t>
+  </si>
+  <si>
+    <t>padding-right --&gt; paddingRight</t>
+  </si>
+  <si>
+    <t>padding-left --&gt; paddingLeft</t>
   </si>
 </sst>
 </file>
@@ -1088,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView topLeftCell="A33" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E46" sqref="A46:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1105,19 +1159,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>24</v>
@@ -1219,13 +1273,13 @@
         <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>124</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1324,13 +1378,13 @@
         <v>63</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>125</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1385,70 +1439,70 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1487,39 +1541,39 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="4" t="s">
         <v>134</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="D24" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>137</v>
       </c>
       <c r="F24" s="1" t="s">
@@ -1527,39 +1581,39 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="4" t="s">
         <v>132</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="4" t="s">
         <v>139</v>
       </c>
       <c r="F26" s="1" t="s">
@@ -1584,36 +1638,36 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1730,7 +1784,7 @@
         <v>65</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>123</v>
@@ -1791,70 +1845,70 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="C41" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="4" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="C42" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="4" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="D43" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1876,53 +1930,53 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1968,7 +2022,7 @@
         <v>129</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>82</v>
@@ -2002,7 +2056,7 @@
         <v>127</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>80</v>
@@ -2019,7 +2073,7 @@
         <v>128</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>81</v>
@@ -2218,7 +2272,7 @@
         <v>155</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2276,39 +2330,39 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="4" t="s">
         <v>135</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E69" s="3" t="s">
+      <c r="D69" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E69" s="4" t="s">
         <v>138</v>
       </c>
       <c r="F69" s="1" t="s">
@@ -2316,23 +2370,23 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E70" s="4" t="s">
         <v>133</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2411,15 +2465,16 @@
     <sortCondition ref="A2:A79"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2429,107 +2484,197 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>189</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: rename theme variables (batch 5)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A10601-7F3D-B947-890C-6141BBA84E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45011F57-4E4D-AF44-9B0D-342D38B8EE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="230">
   <si>
     <t>width</t>
   </si>
@@ -712,6 +712,21 @@
   </si>
   <si>
     <t>padding-left --&gt; paddingLeft</t>
+  </si>
+  <si>
+    <t>padding-top --&gt; paddingTop</t>
+  </si>
+  <si>
+    <t>margin-bottom --&gt; marginBottom</t>
+  </si>
+  <si>
+    <t>margin-left --&gt; marginLeft</t>
+  </si>
+  <si>
+    <t>margin-right --&gt; marginRight</t>
+  </si>
+  <si>
+    <t>margin-top --&gt; marginTop</t>
   </si>
 </sst>
 </file>
@@ -1142,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E46" sqref="A46:E46"/>
+    <sheetView topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E34" sqref="A34:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1689,70 +1704,70 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1981,19 +1996,19 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2471,10 +2486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2677,6 +2692,31 @@
         <v>224</v>
       </c>
     </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>229</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: rename theme variables (batch 5) (#896)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE96999-893E-4649-9031-0801F6031C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6D2265-FB51-7140-ACC7-164B22B64B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout and Theme vars" sheetId="3" r:id="rId1"/>
     <sheet name="Changelog" sheetId="4" r:id="rId2"/>
+    <sheet name="More to rename" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="238">
   <si>
     <t>width</t>
   </si>
@@ -408,9 +409,6 @@
     <t>white-space</t>
   </si>
   <si>
-    <t>maxWidth-content</t>
-  </si>
-  <si>
     <t>borderHorizontal</t>
   </si>
   <si>
@@ -531,9 +529,6 @@
     <t>offset-decoration</t>
   </si>
   <si>
-    <t>width-outline</t>
-  </si>
-  <si>
     <t>outline-style</t>
   </si>
   <si>
@@ -561,9 +556,6 @@
     <t>Maps to the border-left and border-right CSS properties</t>
   </si>
   <si>
-    <t>max-…-width</t>
-  </si>
-  <si>
     <t>border-horizontal</t>
   </si>
   <si>
@@ -658,13 +650,115 @@
   </si>
   <si>
     <t>Changes (theme variables)</t>
+  </si>
+  <si>
+    <t>color-outline --&gt; outlineColor</t>
+  </si>
+  <si>
+    <t>offset-outline --&gt; outlineOffset</t>
+  </si>
+  <si>
+    <t>style-outline --&gt; outlineStyle</t>
+  </si>
+  <si>
+    <t>thickness-outline</t>
+  </si>
+  <si>
+    <t>thickness-outline --&gt; outlineWidth</t>
+  </si>
+  <si>
+    <t>letter-spacing --&gt; letterSpacing</t>
+  </si>
+  <si>
+    <t>line-height --&gt; lineHeight</t>
+  </si>
+  <si>
+    <t>font-family --&gt; fontFamily</t>
+  </si>
+  <si>
+    <t>font-size --&gt; fontSize</t>
+  </si>
+  <si>
+    <t>font-style --&gt; fontStyle</t>
+  </si>
+  <si>
+    <t>margin-horizontal --&gt; marginHorizontal</t>
+  </si>
+  <si>
+    <t>margin-vertical --&gt; marginVertical</t>
+  </si>
+  <si>
+    <t>scroll-horizontal --&gt; overflowX</t>
+  </si>
+  <si>
+    <t>scroll-vertical --&gt; overflowY</t>
+  </si>
+  <si>
+    <t>padding-horizontal --&gt; paddingHorizontal</t>
+  </si>
+  <si>
+    <t>padding-vertical --&gt; paddingVertical</t>
+  </si>
+  <si>
+    <t>padding-bottom --&gt; paddingBottom</t>
+  </si>
+  <si>
+    <t>padding-right --&gt; paddingRight</t>
+  </si>
+  <si>
+    <t>padding-left --&gt; paddingLeft</t>
+  </si>
+  <si>
+    <t>padding-top --&gt; paddingTop</t>
+  </si>
+  <si>
+    <t>margin-bottom --&gt; marginBottom</t>
+  </si>
+  <si>
+    <t>margin-left --&gt; marginLeft</t>
+  </si>
+  <si>
+    <t>margin-right --&gt; marginRight</t>
+  </si>
+  <si>
+    <t>margin-top --&gt; marginTop</t>
+  </si>
+  <si>
+    <t>min-width --&gt; minWidth</t>
+  </si>
+  <si>
+    <t>media-maxWidth-phone</t>
+  </si>
+  <si>
+    <t>media-maxWidth-landscape-phone</t>
+  </si>
+  <si>
+    <t>media-maxWidth-tablet</t>
+  </si>
+  <si>
+    <t>media-maxWidth-desktop</t>
+  </si>
+  <si>
+    <t>media-maxWidth-large-desktop</t>
+  </si>
+  <si>
+    <t>max-content-width</t>
+  </si>
+  <si>
+    <t>max-width --&gt; maxWidth</t>
+  </si>
+  <si>
+    <t>max-height --&gt; maxHeight</t>
+  </si>
+  <si>
+    <t>min-height --&gt; minHeight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -711,6 +805,13 @@
       <name val="Aptos Display"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -744,12 +845,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1088,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E37" sqref="A37:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1105,19 +1207,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>24</v>
@@ -1210,22 +1312,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1284,7 +1386,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>77</v>
@@ -1293,7 +1395,7 @@
         <v>78</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1315,22 +1417,22 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1385,70 +1487,70 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1487,80 +1589,80 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C23" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>134</v>
+      <c r="E23" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>137</v>
+      <c r="D24" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>132</v>
+      <c r="E25" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>139</v>
+      <c r="E26" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>110</v>
@@ -1584,36 +1686,36 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1635,141 +1737,141 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>123</v>
+      <c r="D36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1791,71 +1893,71 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>144</v>
-      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>140</v>
+      <c r="A43" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1876,70 +1978,70 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1948,7 +2050,7 @@
         <v>19</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>79</v>
@@ -1957,7 +2059,7 @@
         <v>19</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1965,16 +2067,16 @@
         <v>22</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1982,7 +2084,7 @@
         <v>23</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>83</v>
@@ -1991,7 +2093,7 @@
         <v>84</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1999,16 +2101,16 @@
         <v>20</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2016,16 +2118,16 @@
         <v>21</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2050,7 +2152,7 @@
         <v>41</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>99</v>
@@ -2059,7 +2161,7 @@
         <v>41</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2115,70 +2217,70 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2203,22 +2305,22 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B64" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="D64" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2276,63 +2378,63 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E68" s="3" t="s">
-        <v>135</v>
+      <c r="E68" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C69" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>138</v>
+      <c r="D69" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C70" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>133</v>
+      <c r="E70" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2411,15 +2513,16 @@
     <sortCondition ref="A2:A79"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A48"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2429,107 +2532,290 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114F83F-F3AF-0B4F-A4C1-A92AE23C196B}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: rename theme variables (batch 6)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6D2265-FB51-7140-ACC7-164B22B64B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACC1856-CD2A-6647-B60E-7D57A1D94611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="303">
   <si>
     <t>width</t>
   </si>
@@ -752,6 +752,201 @@
   </si>
   <si>
     <t>min-height --&gt; minHeight</t>
+  </si>
+  <si>
+    <t>radius --&gt; borderRadius</t>
+  </si>
+  <si>
+    <t>border-radius-end-start --&gt; borderRadiusEndStart</t>
+  </si>
+  <si>
+    <t>border-radius-end-end --&gt; borderRadiusEndEnd</t>
+  </si>
+  <si>
+    <t>border-radius-start-start --&gt; borderRadiusStartStart</t>
+  </si>
+  <si>
+    <t>border-radius-start-end --&gt; borderRadiusStartEnd</t>
+  </si>
+  <si>
+    <t>color-border-left</t>
+  </si>
+  <si>
+    <t>borderLeftColor</t>
+  </si>
+  <si>
+    <t>border-left-style</t>
+  </si>
+  <si>
+    <t>borderLeftStyle</t>
+  </si>
+  <si>
+    <t>border-left-width</t>
+  </si>
+  <si>
+    <t>borderLeftWidth</t>
+  </si>
+  <si>
+    <t>border-left-color</t>
+  </si>
+  <si>
+    <t>border-right-color</t>
+  </si>
+  <si>
+    <t>style-border-left</t>
+  </si>
+  <si>
+    <t>thickness-border-left</t>
+  </si>
+  <si>
+    <t>border-right-style</t>
+  </si>
+  <si>
+    <t>border-right-width</t>
+  </si>
+  <si>
+    <t>color-border-right</t>
+  </si>
+  <si>
+    <t>style-border-right</t>
+  </si>
+  <si>
+    <t>thickness-border-right</t>
+  </si>
+  <si>
+    <t>borderRightColor</t>
+  </si>
+  <si>
+    <t>borderRightStyle</t>
+  </si>
+  <si>
+    <t>borderRightWidth</t>
+  </si>
+  <si>
+    <t>border-bottom-color</t>
+  </si>
+  <si>
+    <t>border-bottom-style</t>
+  </si>
+  <si>
+    <t>border-bottom-width</t>
+  </si>
+  <si>
+    <t>color-border-bottom</t>
+  </si>
+  <si>
+    <t>style-border-bottom</t>
+  </si>
+  <si>
+    <t>thickness-border-bottom</t>
+  </si>
+  <si>
+    <t>borderBottomColor</t>
+  </si>
+  <si>
+    <t>borderBottomStyle</t>
+  </si>
+  <si>
+    <t>borderBottomWidth</t>
+  </si>
+  <si>
+    <t>border-top-color</t>
+  </si>
+  <si>
+    <t>border-top-style</t>
+  </si>
+  <si>
+    <t>border-top-width</t>
+  </si>
+  <si>
+    <t>color-border-top</t>
+  </si>
+  <si>
+    <t>style-border-top</t>
+  </si>
+  <si>
+    <t>thickness-border-top</t>
+  </si>
+  <si>
+    <t>borderTopColor</t>
+  </si>
+  <si>
+    <t>borderTopStyle</t>
+  </si>
+  <si>
+    <t>borderTopWidth</t>
+  </si>
+  <si>
+    <t>color-border-bottom --&gt; borderBottomColor</t>
+  </si>
+  <si>
+    <t>style-border-bottom --&gt; borderBottomStyle</t>
+  </si>
+  <si>
+    <t>thickness-border-bottom --&gt; borderBottomThickness</t>
+  </si>
+  <si>
+    <t>border-bottom --&gt; borderBottom</t>
+  </si>
+  <si>
+    <t>color-border-horizontal</t>
+  </si>
+  <si>
+    <t>style-border-horizontal</t>
+  </si>
+  <si>
+    <t>thickness-border-horizontal</t>
+  </si>
+  <si>
+    <t>borderHorizontalColor</t>
+  </si>
+  <si>
+    <t>borderHorizontalStyle</t>
+  </si>
+  <si>
+    <t>borderHorizontalWidth</t>
+  </si>
+  <si>
+    <t>color-border-vertical</t>
+  </si>
+  <si>
+    <t>style-border-vertical</t>
+  </si>
+  <si>
+    <t>thickness-border-vertical</t>
+  </si>
+  <si>
+    <t>borderVerticalColor</t>
+  </si>
+  <si>
+    <t>borderVerticalStyle</t>
+  </si>
+  <si>
+    <t>borderVerticalWidth</t>
+  </si>
+  <si>
+    <t>thickness-border-horizontal --&gt; borderHorizontalWidth</t>
+  </si>
+  <si>
+    <t>style-border-horizontal --&gt; borderHorizontalStyle</t>
+  </si>
+  <si>
+    <t>color-border-horizontal --&gt; borderHorizontalColor</t>
+  </si>
+  <si>
+    <t>border-horizontal --&gt; borderHorizontal</t>
+  </si>
+  <si>
+    <t>thickness-border-vertical --&gt; borderVerticalWidth</t>
+  </si>
+  <si>
+    <t>style-border-vertical --&gt; borderVerticalStyle</t>
+  </si>
+  <si>
+    <t>color-border-vertical --&gt; borderVerticalColor</t>
+  </si>
+  <si>
+    <t>border-vertical --&gt; borderVertical</t>
   </si>
 </sst>
 </file>
@@ -1188,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E37" sqref="A37:E37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1199,7 +1394,7 @@
     <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="94.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
@@ -1277,1240 +1472,1546 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
+      <c r="A6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>123</v>
+      <c r="A7" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>171</v>
+        <v>63</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
+      <c r="A8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>177</v>
+      <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>110</v>
+      <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>10</v>
+      <c r="A27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>54</v>
+        <v>124</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>118</v>
+        <v>289</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>56</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>32</v>
+        <v>290</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>32</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>95</v>
+        <v>291</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>37</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>157</v>
+        <v>3</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>140</v>
+        <v>3</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>141</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>145</v>
+        <v>33</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>164</v>
+        <v>63</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>144</v>
+        <v>91</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>145</v>
+        <v>133</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>143</v>
+        <v>43</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>163</v>
+        <v>100</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>139</v>
+        <v>26</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>156</v>
+        <v>63</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>139</v>
+        <v>131</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>25</v>
+        <v>138</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>25</v>
+        <v>138</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>125</v>
+      <c r="A49" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>128</v>
+      <c r="A50" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>129</v>
+      <c r="A51" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>126</v>
+      <c r="A52" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>127</v>
+      <c r="A53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>135</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>149</v>
+        <v>25</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>149</v>
+        <v>25</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>161</v>
+        <v>25</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>149</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C82" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D82" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E82" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C83" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D83" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E83" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C84" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D84" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E84" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C85" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D67" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E67" s="4" t="s">
+      <c r="D85" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E85" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="F85" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D68" s="4" t="s">
+      <c r="C86" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D86" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E86" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F86" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C87" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D87" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E87" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F87" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D70" s="4" t="s">
+      <c r="C88" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D88" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E88" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F88" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C89" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D71" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E71" s="4" t="s">
+      <c r="D89" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E89" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C90" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D90" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E90" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C91" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E73" s="4" t="s">
+      <c r="D91" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E91" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F91" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C92" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D92" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E92" s="4" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F79">
-    <sortCondition ref="A2:A79"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F97">
+    <sortCondition ref="A2:A97"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2519,15 +3020,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A48"/>
+  <dimension ref="A1:A64"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A44" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -2768,6 +3269,86 @@
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2777,10 +3358,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114F83F-F3AF-0B4F-A4C1-A92AE23C196B}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2818,6 +3399,11 @@
         <v>234</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>238</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: rename theme variables (batch 6) (#899)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6D2265-FB51-7140-ACC7-164B22B64B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACC1856-CD2A-6647-B60E-7D57A1D94611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="303">
   <si>
     <t>width</t>
   </si>
@@ -752,6 +752,201 @@
   </si>
   <si>
     <t>min-height --&gt; minHeight</t>
+  </si>
+  <si>
+    <t>radius --&gt; borderRadius</t>
+  </si>
+  <si>
+    <t>border-radius-end-start --&gt; borderRadiusEndStart</t>
+  </si>
+  <si>
+    <t>border-radius-end-end --&gt; borderRadiusEndEnd</t>
+  </si>
+  <si>
+    <t>border-radius-start-start --&gt; borderRadiusStartStart</t>
+  </si>
+  <si>
+    <t>border-radius-start-end --&gt; borderRadiusStartEnd</t>
+  </si>
+  <si>
+    <t>color-border-left</t>
+  </si>
+  <si>
+    <t>borderLeftColor</t>
+  </si>
+  <si>
+    <t>border-left-style</t>
+  </si>
+  <si>
+    <t>borderLeftStyle</t>
+  </si>
+  <si>
+    <t>border-left-width</t>
+  </si>
+  <si>
+    <t>borderLeftWidth</t>
+  </si>
+  <si>
+    <t>border-left-color</t>
+  </si>
+  <si>
+    <t>border-right-color</t>
+  </si>
+  <si>
+    <t>style-border-left</t>
+  </si>
+  <si>
+    <t>thickness-border-left</t>
+  </si>
+  <si>
+    <t>border-right-style</t>
+  </si>
+  <si>
+    <t>border-right-width</t>
+  </si>
+  <si>
+    <t>color-border-right</t>
+  </si>
+  <si>
+    <t>style-border-right</t>
+  </si>
+  <si>
+    <t>thickness-border-right</t>
+  </si>
+  <si>
+    <t>borderRightColor</t>
+  </si>
+  <si>
+    <t>borderRightStyle</t>
+  </si>
+  <si>
+    <t>borderRightWidth</t>
+  </si>
+  <si>
+    <t>border-bottom-color</t>
+  </si>
+  <si>
+    <t>border-bottom-style</t>
+  </si>
+  <si>
+    <t>border-bottom-width</t>
+  </si>
+  <si>
+    <t>color-border-bottom</t>
+  </si>
+  <si>
+    <t>style-border-bottom</t>
+  </si>
+  <si>
+    <t>thickness-border-bottom</t>
+  </si>
+  <si>
+    <t>borderBottomColor</t>
+  </si>
+  <si>
+    <t>borderBottomStyle</t>
+  </si>
+  <si>
+    <t>borderBottomWidth</t>
+  </si>
+  <si>
+    <t>border-top-color</t>
+  </si>
+  <si>
+    <t>border-top-style</t>
+  </si>
+  <si>
+    <t>border-top-width</t>
+  </si>
+  <si>
+    <t>color-border-top</t>
+  </si>
+  <si>
+    <t>style-border-top</t>
+  </si>
+  <si>
+    <t>thickness-border-top</t>
+  </si>
+  <si>
+    <t>borderTopColor</t>
+  </si>
+  <si>
+    <t>borderTopStyle</t>
+  </si>
+  <si>
+    <t>borderTopWidth</t>
+  </si>
+  <si>
+    <t>color-border-bottom --&gt; borderBottomColor</t>
+  </si>
+  <si>
+    <t>style-border-bottom --&gt; borderBottomStyle</t>
+  </si>
+  <si>
+    <t>thickness-border-bottom --&gt; borderBottomThickness</t>
+  </si>
+  <si>
+    <t>border-bottom --&gt; borderBottom</t>
+  </si>
+  <si>
+    <t>color-border-horizontal</t>
+  </si>
+  <si>
+    <t>style-border-horizontal</t>
+  </si>
+  <si>
+    <t>thickness-border-horizontal</t>
+  </si>
+  <si>
+    <t>borderHorizontalColor</t>
+  </si>
+  <si>
+    <t>borderHorizontalStyle</t>
+  </si>
+  <si>
+    <t>borderHorizontalWidth</t>
+  </si>
+  <si>
+    <t>color-border-vertical</t>
+  </si>
+  <si>
+    <t>style-border-vertical</t>
+  </si>
+  <si>
+    <t>thickness-border-vertical</t>
+  </si>
+  <si>
+    <t>borderVerticalColor</t>
+  </si>
+  <si>
+    <t>borderVerticalStyle</t>
+  </si>
+  <si>
+    <t>borderVerticalWidth</t>
+  </si>
+  <si>
+    <t>thickness-border-horizontal --&gt; borderHorizontalWidth</t>
+  </si>
+  <si>
+    <t>style-border-horizontal --&gt; borderHorizontalStyle</t>
+  </si>
+  <si>
+    <t>color-border-horizontal --&gt; borderHorizontalColor</t>
+  </si>
+  <si>
+    <t>border-horizontal --&gt; borderHorizontal</t>
+  </si>
+  <si>
+    <t>thickness-border-vertical --&gt; borderVerticalWidth</t>
+  </si>
+  <si>
+    <t>style-border-vertical --&gt; borderVerticalStyle</t>
+  </si>
+  <si>
+    <t>color-border-vertical --&gt; borderVerticalColor</t>
+  </si>
+  <si>
+    <t>border-vertical --&gt; borderVertical</t>
   </si>
 </sst>
 </file>
@@ -1188,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E37" sqref="A37:E37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1199,7 +1394,7 @@
     <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="94.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
@@ -1277,1240 +1472,1546 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
+      <c r="A6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>123</v>
+      <c r="A7" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>171</v>
+        <v>63</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
+      <c r="A8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>177</v>
+      <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>110</v>
+      <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>10</v>
+      <c r="A27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>54</v>
+        <v>124</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>118</v>
+        <v>289</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>56</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>32</v>
+        <v>290</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>32</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>95</v>
+        <v>291</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>37</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>157</v>
+        <v>3</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>140</v>
+        <v>3</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>141</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>145</v>
+        <v>33</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>164</v>
+        <v>63</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>144</v>
+        <v>91</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>145</v>
+        <v>133</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>143</v>
+        <v>43</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>163</v>
+        <v>100</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>139</v>
+        <v>26</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>156</v>
+        <v>63</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>139</v>
+        <v>131</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>25</v>
+        <v>138</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>25</v>
+        <v>138</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>125</v>
+      <c r="A49" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>128</v>
+      <c r="A50" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>129</v>
+      <c r="A51" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>126</v>
+      <c r="A52" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>127</v>
+      <c r="A53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>135</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>149</v>
+        <v>25</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>149</v>
+        <v>25</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>161</v>
+        <v>25</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>149</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C82" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D82" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E82" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C83" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D83" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E83" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C84" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D84" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E84" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C85" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D67" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E67" s="4" t="s">
+      <c r="D85" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E85" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="F85" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D68" s="4" t="s">
+      <c r="C86" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D86" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E86" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F86" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C87" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D87" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E87" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F87" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D70" s="4" t="s">
+      <c r="C88" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D88" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E88" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F88" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C89" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D71" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E71" s="4" t="s">
+      <c r="D89" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E89" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C90" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D90" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E90" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C91" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E73" s="4" t="s">
+      <c r="D91" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E91" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F91" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C92" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D92" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E92" s="4" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F79">
-    <sortCondition ref="A2:A79"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F97">
+    <sortCondition ref="A2:A97"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2519,15 +3020,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A48"/>
+  <dimension ref="A1:A64"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A44" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -2768,6 +3269,86 @@
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2777,10 +3358,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114F83F-F3AF-0B4F-A4C1-A92AE23C196B}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2818,6 +3399,11 @@
         <v>234</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>238</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: rename theme variables (batch 7)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D46E27E-1DD9-9444-A7A2-BFE27565A5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1390F0C7-7916-D841-A9FB-4A21D057465A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="319">
   <si>
     <t>width</t>
   </si>
@@ -983,6 +983,18 @@
   </si>
   <si>
     <t>border-top --&gt; borderTop</t>
+  </si>
+  <si>
+    <t>thickness-border --&gt; borderWidth</t>
+  </si>
+  <si>
+    <t>style-border --&gt; borderStyle</t>
+  </si>
+  <si>
+    <t>color-text: review</t>
+  </si>
+  <si>
+    <t>color-border --&gt; borderColor</t>
   </si>
 </sst>
 </file>
@@ -1422,7 +1434,7 @@
   <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="E9" sqref="A9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1576,19 +1588,19 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1800,36 +1812,36 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="4" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3056,10 +3068,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A76"/>
+  <dimension ref="A1:A79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3447,6 +3459,21 @@
         <v>314</v>
       </c>
     </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3454,10 +3481,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114F83F-F3AF-0B4F-A4C1-A92AE23C196B}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3500,6 +3527,11 @@
         <v>238</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>317</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: rename theme variables (batch 7) (#902)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACC1856-CD2A-6647-B60E-7D57A1D94611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1390F0C7-7916-D841-A9FB-4A21D057465A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout and Theme vars" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="319">
   <si>
     <t>width</t>
   </si>
@@ -947,6 +947,54 @@
   </si>
   <si>
     <t>border-vertical --&gt; borderVertical</t>
+  </si>
+  <si>
+    <t>thickness-border-left --&gt; borderLeftWidth</t>
+  </si>
+  <si>
+    <t>style-border-left --&gt; borderLeftStyle</t>
+  </si>
+  <si>
+    <t>color-border-left --&gt; borderLeftColor</t>
+  </si>
+  <si>
+    <t>border-left --&gt; borderLeft</t>
+  </si>
+  <si>
+    <t>thickness-border-right --&gt; borderRightWidth</t>
+  </si>
+  <si>
+    <t>style-border-right --&gt; borderRigthStyle</t>
+  </si>
+  <si>
+    <t>color-border-right --&gt; borderRigthColor</t>
+  </si>
+  <si>
+    <t>border-right --&gt; borderRigth</t>
+  </si>
+  <si>
+    <t>thickness-border-top --&gt; borderTopWidth</t>
+  </si>
+  <si>
+    <t>style-border-top --&gt; borderTopStyle</t>
+  </si>
+  <si>
+    <t>color-border-top --&gt; borderTopColor</t>
+  </si>
+  <si>
+    <t>border-top --&gt; borderTop</t>
+  </si>
+  <si>
+    <t>thickness-border --&gt; borderWidth</t>
+  </si>
+  <si>
+    <t>style-border --&gt; borderStyle</t>
+  </si>
+  <si>
+    <t>color-text: review</t>
+  </si>
+  <si>
+    <t>color-border --&gt; borderColor</t>
   </si>
 </sst>
 </file>
@@ -1385,8 +1433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E9" sqref="A9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1540,19 +1588,19 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1628,240 +1676,240 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="A15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="4" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="A16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="4" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="A17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="A19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="4" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="A20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="4" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="A21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="4" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="4" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="A25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="4" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="A26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="4" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="A27" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="4" t="s">
         <v>278</v>
       </c>
     </row>
@@ -3020,10 +3068,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A64"/>
+  <dimension ref="A1:A79"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3351,6 +3399,81 @@
         <v>302</v>
       </c>
     </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3358,10 +3481,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114F83F-F3AF-0B4F-A4C1-A92AE23C196B}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3404,6 +3527,11 @@
         <v>238</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>317</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: rename theme variables (batch 8) (#905)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1390F0C7-7916-D841-A9FB-4A21D057465A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF89AE9-F8EE-644A-95A9-4E7BBAD0B758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="327">
   <si>
     <t>width</t>
   </si>
@@ -995,13 +995,37 @@
   </si>
   <si>
     <t>color-border --&gt; borderColor</t>
+  </si>
+  <si>
+    <t>color-bg --&gt; backgroundColor</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>media-maxWidth-phone --&gt; maxWidth-phone</t>
+  </si>
+  <si>
+    <t>media-maxWidth-landscape-phone --&gt; maxWidth-landscape-phone</t>
+  </si>
+  <si>
+    <t>media-maxWidth-tablet --&gt; maxWidth-tablet</t>
+  </si>
+  <si>
+    <t>media-maxWidth-desktop --&gt; maxWidth-desktop</t>
+  </si>
+  <si>
+    <t>media-maxWidth-large-desktop --&gt; maxWidth-large-desktop</t>
+  </si>
+  <si>
+    <t>max-content-width --&gt; maxWidth-content</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1019,19 +1043,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Display"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
       <name val="Aptos Display"/>
       <scheme val="major"/>
     </font>
@@ -1056,17 +1067,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1083,22 +1089,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1433,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="A9:E9"/>
+    <sheetView topLeftCell="A47" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1469,16 +1472,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1486,16 +1489,16 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>98</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1503,121 +1506,121 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="A6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="A8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>123</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1625,308 +1628,308 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="A11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="A12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="A13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="A15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="A16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="A17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="A19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="A20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="A21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="A25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="A26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="A27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>124</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1934,223 +1937,223 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="A29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="A30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="A31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="3" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="4" t="s">
+      <c r="C41" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="3" t="s">
         <v>133</v>
       </c>
       <c r="F41" s="1" t="s">
@@ -2158,19 +2161,19 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="3" t="s">
         <v>136</v>
       </c>
       <c r="F42" s="1" t="s">
@@ -2178,19 +2181,19 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="4" t="s">
+      <c r="C43" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="3" t="s">
         <v>131</v>
       </c>
       <c r="F43" s="1" t="s">
@@ -2198,19 +2201,19 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E44" s="4" t="s">
+      <c r="D44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>138</v>
       </c>
       <c r="F44" s="1" t="s">
@@ -2218,172 +2221,172 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E49" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F54" s="1" t="s">
@@ -2391,461 +2394,461 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E58" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="3" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E60" s="3" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E62" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E66" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E67" s="3" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E68" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E69" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E70" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="E71" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E72" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E73" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E74" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C75" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D75" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E75" s="4" t="s">
+      <c r="E75" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C76" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D76" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E76" s="4" t="s">
+      <c r="E76" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C77" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E77" s="4" t="s">
+      <c r="E77" s="3" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C78" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E78" s="4" t="s">
+      <c r="E78" s="3" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C79" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E79" s="4" t="s">
+      <c r="E79" s="3" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="C80" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E80" s="4" t="s">
+      <c r="E80" s="3" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E81" s="3" t="s">
         <v>55</v>
       </c>
       <c r="F81" s="1" t="s">
@@ -2853,19 +2856,19 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C82" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="D82" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E82" s="4" t="s">
+      <c r="E82" s="3" t="s">
         <v>154</v>
       </c>
       <c r="F82" s="1" t="s">
@@ -2873,53 +2876,53 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="C83" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D83" s="4" t="s">
+      <c r="D83" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="E83" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C84" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="D84" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E84" s="4" t="s">
+      <c r="E84" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="C85" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D85" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E85" s="4" t="s">
+      <c r="D85" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>53</v>
       </c>
       <c r="F85" s="1" t="s">
@@ -2927,19 +2930,19 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C86" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D86" s="4" t="s">
+      <c r="C86" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="E86" s="3" t="s">
         <v>134</v>
       </c>
       <c r="F86" s="1" t="s">
@@ -2947,19 +2950,19 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C87" s="4" t="s">
+      <c r="C87" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D87" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="E87" s="4" t="s">
+      <c r="E87" s="3" t="s">
         <v>137</v>
       </c>
       <c r="F87" s="1" t="s">
@@ -2967,19 +2970,19 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C88" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D88" s="4" t="s">
+      <c r="C88" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D88" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E88" s="4" t="s">
+      <c r="E88" s="3" t="s">
         <v>132</v>
       </c>
       <c r="F88" s="1" t="s">
@@ -2987,53 +2990,53 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D89" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E89" s="4" t="s">
+      <c r="D89" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E89" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C90" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D90" s="4" t="s">
+      <c r="D90" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E90" s="4" t="s">
+      <c r="E90" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C91" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D91" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E91" s="4" t="s">
+      <c r="D91" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E91" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F91" s="1" t="s">
@@ -3041,19 +3044,19 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
+      <c r="A92" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C92" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D92" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E92" s="4" t="s">
+      <c r="E92" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3068,15 +3071,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A79"/>
+  <dimension ref="A1:A87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -3472,6 +3475,46 @@
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>318</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -3484,7 +3527,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3503,12 +3546,12 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>232</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: rename theme variables (batch 9)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF89AE9-F8EE-644A-95A9-4E7BBAD0B758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1F8C3A-9F6A-EA4A-A5D8-A6FA8B6AAA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="332">
   <si>
     <t>width</t>
   </si>
@@ -1019,6 +1019,21 @@
   </si>
   <si>
     <t>max-content-width --&gt; maxWidth-content</t>
+  </si>
+  <si>
+    <t>textColor-primary</t>
+  </si>
+  <si>
+    <t>textColor-attention</t>
+  </si>
+  <si>
+    <t>textColor-subtitle</t>
+  </si>
+  <si>
+    <t>textColor-secondary</t>
+  </si>
+  <si>
+    <t>shadow-md --&gt; boxShadow-md</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -3073,8 +3088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
   <dimension ref="A1:A87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3524,10 +3539,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114F83F-F3AF-0B4F-A4C1-A92AE23C196B}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3575,6 +3590,31 @@
         <v>317</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>331</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: rename theme variables (batch 9) (#908)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF89AE9-F8EE-644A-95A9-4E7BBAD0B758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1F8C3A-9F6A-EA4A-A5D8-A6FA8B6AAA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="332">
   <si>
     <t>width</t>
   </si>
@@ -1019,6 +1019,21 @@
   </si>
   <si>
     <t>max-content-width --&gt; maxWidth-content</t>
+  </si>
+  <si>
+    <t>textColor-primary</t>
+  </si>
+  <si>
+    <t>textColor-attention</t>
+  </si>
+  <si>
+    <t>textColor-subtitle</t>
+  </si>
+  <si>
+    <t>textColor-secondary</t>
+  </si>
+  <si>
+    <t>shadow-md --&gt; boxShadow-md</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -3073,8 +3088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
   <dimension ref="A1:A87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3524,10 +3539,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114F83F-F3AF-0B4F-A4C1-A92AE23C196B}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3575,6 +3590,31 @@
         <v>317</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>331</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
build: prepare to release v0.8.0
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1F8C3A-9F6A-EA4A-A5D8-A6FA8B6AAA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEEB7A1-6D8E-D84D-9BFB-F5A9AE3A6C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Layout and Theme vars" sheetId="3" r:id="rId1"/>
-    <sheet name="Changelog" sheetId="4" r:id="rId2"/>
-    <sheet name="More to rename" sheetId="5" r:id="rId3"/>
+    <sheet name="Changelog" sheetId="4" r:id="rId1"/>
+    <sheet name="Layout and Theme vars" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="353">
   <si>
     <t>width</t>
   </si>
@@ -589,144 +588,12 @@
     <t>scroll-vertical</t>
   </si>
   <si>
-    <t>Introduce borderHorizontal</t>
-  </si>
-  <si>
-    <t>Introduce borderVertical</t>
-  </si>
-  <si>
-    <t>italic --&gt; fontStyle</t>
-  </si>
-  <si>
-    <t>shadow --&gt; boxShadow</t>
-  </si>
-  <si>
-    <t>borderThickness --&gt; borderWidth</t>
-  </si>
-  <si>
-    <t>horizontalMargin --&gt; marginHorizontal</t>
-  </si>
-  <si>
-    <t>verticalMargin --&gt; marginVertical</t>
-  </si>
-  <si>
-    <t>horizontalPadding --&gt; paddingHorizontal</t>
-  </si>
-  <si>
-    <t>verticalPadding --&gt; paddingVertical</t>
-  </si>
-  <si>
     <t>(existing theme vars: offset-decoration)</t>
   </si>
   <si>
-    <t>offset-decoration --&gt; textUnderlineOffset</t>
-  </si>
-  <si>
-    <t>text-transform --&gt; textTransform</t>
-  </si>
-  <si>
-    <t>transform-text --&gt; textTransform</t>
-  </si>
-  <si>
-    <t>"transform-" --&gt; textTransform</t>
-  </si>
-  <si>
-    <t>thickness-decoration --&gt; textDecorationThickness</t>
-  </si>
-  <si>
-    <t>style-decoration --&gt; textDecorationStyle</t>
-  </si>
-  <si>
-    <t>line-decoration --&gt; textDecorationLine</t>
-  </si>
-  <si>
-    <t>color-decoration --&gt; textDecorationColor</t>
-  </si>
-  <si>
-    <t>text-decoration --&gt; textDecoration</t>
-  </si>
-  <si>
-    <t>Changes (layout properties)</t>
-  </si>
-  <si>
-    <t>Changes (theme variables)</t>
-  </si>
-  <si>
-    <t>color-outline --&gt; outlineColor</t>
-  </si>
-  <si>
-    <t>offset-outline --&gt; outlineOffset</t>
-  </si>
-  <si>
-    <t>style-outline --&gt; outlineStyle</t>
-  </si>
-  <si>
     <t>thickness-outline</t>
   </si>
   <si>
-    <t>thickness-outline --&gt; outlineWidth</t>
-  </si>
-  <si>
-    <t>letter-spacing --&gt; letterSpacing</t>
-  </si>
-  <si>
-    <t>line-height --&gt; lineHeight</t>
-  </si>
-  <si>
-    <t>font-family --&gt; fontFamily</t>
-  </si>
-  <si>
-    <t>font-size --&gt; fontSize</t>
-  </si>
-  <si>
-    <t>font-style --&gt; fontStyle</t>
-  </si>
-  <si>
-    <t>margin-horizontal --&gt; marginHorizontal</t>
-  </si>
-  <si>
-    <t>margin-vertical --&gt; marginVertical</t>
-  </si>
-  <si>
-    <t>scroll-horizontal --&gt; overflowX</t>
-  </si>
-  <si>
-    <t>scroll-vertical --&gt; overflowY</t>
-  </si>
-  <si>
-    <t>padding-horizontal --&gt; paddingHorizontal</t>
-  </si>
-  <si>
-    <t>padding-vertical --&gt; paddingVertical</t>
-  </si>
-  <si>
-    <t>padding-bottom --&gt; paddingBottom</t>
-  </si>
-  <si>
-    <t>padding-right --&gt; paddingRight</t>
-  </si>
-  <si>
-    <t>padding-left --&gt; paddingLeft</t>
-  </si>
-  <si>
-    <t>padding-top --&gt; paddingTop</t>
-  </si>
-  <si>
-    <t>margin-bottom --&gt; marginBottom</t>
-  </si>
-  <si>
-    <t>margin-left --&gt; marginLeft</t>
-  </si>
-  <si>
-    <t>margin-right --&gt; marginRight</t>
-  </si>
-  <si>
-    <t>margin-top --&gt; marginTop</t>
-  </si>
-  <si>
-    <t>min-width --&gt; minWidth</t>
-  </si>
-  <si>
     <t>media-maxWidth-phone</t>
   </si>
   <si>
@@ -745,30 +612,6 @@
     <t>max-content-width</t>
   </si>
   <si>
-    <t>max-width --&gt; maxWidth</t>
-  </si>
-  <si>
-    <t>max-height --&gt; maxHeight</t>
-  </si>
-  <si>
-    <t>min-height --&gt; minHeight</t>
-  </si>
-  <si>
-    <t>radius --&gt; borderRadius</t>
-  </si>
-  <si>
-    <t>border-radius-end-start --&gt; borderRadiusEndStart</t>
-  </si>
-  <si>
-    <t>border-radius-end-end --&gt; borderRadiusEndEnd</t>
-  </si>
-  <si>
-    <t>border-radius-start-start --&gt; borderRadiusStartStart</t>
-  </si>
-  <si>
-    <t>border-radius-start-end --&gt; borderRadiusStartEnd</t>
-  </si>
-  <si>
     <t>color-border-left</t>
   </si>
   <si>
@@ -877,18 +720,6 @@
     <t>borderTopWidth</t>
   </si>
   <si>
-    <t>color-border-bottom --&gt; borderBottomColor</t>
-  </si>
-  <si>
-    <t>style-border-bottom --&gt; borderBottomStyle</t>
-  </si>
-  <si>
-    <t>thickness-border-bottom --&gt; borderBottomThickness</t>
-  </si>
-  <si>
-    <t>border-bottom --&gt; borderBottom</t>
-  </si>
-  <si>
     <t>color-border-horizontal</t>
   </si>
   <si>
@@ -925,102 +756,6 @@
     <t>borderVerticalWidth</t>
   </si>
   <si>
-    <t>thickness-border-horizontal --&gt; borderHorizontalWidth</t>
-  </si>
-  <si>
-    <t>style-border-horizontal --&gt; borderHorizontalStyle</t>
-  </si>
-  <si>
-    <t>color-border-horizontal --&gt; borderHorizontalColor</t>
-  </si>
-  <si>
-    <t>border-horizontal --&gt; borderHorizontal</t>
-  </si>
-  <si>
-    <t>thickness-border-vertical --&gt; borderVerticalWidth</t>
-  </si>
-  <si>
-    <t>style-border-vertical --&gt; borderVerticalStyle</t>
-  </si>
-  <si>
-    <t>color-border-vertical --&gt; borderVerticalColor</t>
-  </si>
-  <si>
-    <t>border-vertical --&gt; borderVertical</t>
-  </si>
-  <si>
-    <t>thickness-border-left --&gt; borderLeftWidth</t>
-  </si>
-  <si>
-    <t>style-border-left --&gt; borderLeftStyle</t>
-  </si>
-  <si>
-    <t>color-border-left --&gt; borderLeftColor</t>
-  </si>
-  <si>
-    <t>border-left --&gt; borderLeft</t>
-  </si>
-  <si>
-    <t>thickness-border-right --&gt; borderRightWidth</t>
-  </si>
-  <si>
-    <t>style-border-right --&gt; borderRigthStyle</t>
-  </si>
-  <si>
-    <t>color-border-right --&gt; borderRigthColor</t>
-  </si>
-  <si>
-    <t>border-right --&gt; borderRigth</t>
-  </si>
-  <si>
-    <t>thickness-border-top --&gt; borderTopWidth</t>
-  </si>
-  <si>
-    <t>style-border-top --&gt; borderTopStyle</t>
-  </si>
-  <si>
-    <t>color-border-top --&gt; borderTopColor</t>
-  </si>
-  <si>
-    <t>border-top --&gt; borderTop</t>
-  </si>
-  <si>
-    <t>thickness-border --&gt; borderWidth</t>
-  </si>
-  <si>
-    <t>style-border --&gt; borderStyle</t>
-  </si>
-  <si>
-    <t>color-text: review</t>
-  </si>
-  <si>
-    <t>color-border --&gt; borderColor</t>
-  </si>
-  <si>
-    <t>color-bg --&gt; backgroundColor</t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
-    <t>media-maxWidth-phone --&gt; maxWidth-phone</t>
-  </si>
-  <si>
-    <t>media-maxWidth-landscape-phone --&gt; maxWidth-landscape-phone</t>
-  </si>
-  <si>
-    <t>media-maxWidth-tablet --&gt; maxWidth-tablet</t>
-  </si>
-  <si>
-    <t>media-maxWidth-desktop --&gt; maxWidth-desktop</t>
-  </si>
-  <si>
-    <t>media-maxWidth-large-desktop --&gt; maxWidth-large-desktop</t>
-  </si>
-  <si>
-    <t>max-content-width --&gt; maxWidth-content</t>
-  </si>
-  <si>
     <t>textColor-primary</t>
   </si>
   <si>
@@ -1033,14 +768,341 @@
     <t>textColor-secondary</t>
   </si>
   <si>
-    <t>shadow-md --&gt; boxShadow-md</t>
+    <t>Old name</t>
+  </si>
+  <si>
+    <t>New name</t>
+  </si>
+  <si>
+    <t>Layout (inline component) properties</t>
+  </si>
+  <si>
+    <t>Theme variable prefixes</t>
+  </si>
+  <si>
+    <t>App-bound theme variables</t>
+  </si>
+  <si>
+    <t>boolean changed to "normal" or "italic"</t>
+  </si>
+  <si>
+    <t>transform-text</t>
+  </si>
+  <si>
+    <t>transform</t>
+  </si>
+  <si>
+    <t>border-radius-end-end</t>
+  </si>
+  <si>
+    <t>border-radius-start-end</t>
+  </si>
+  <si>
+    <t>borderBottomThickness</t>
+  </si>
+  <si>
+    <t>borderRigthStyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> borderRigthColor</t>
+  </si>
+  <si>
+    <t>borderRigth</t>
+  </si>
+  <si>
+    <t>maxWidth-phone</t>
+  </si>
+  <si>
+    <t>maxWidth-landscape-phone</t>
+  </si>
+  <si>
+    <t>maxWidth-tablet</t>
+  </si>
+  <si>
+    <t>maxWidth-desktop</t>
+  </si>
+  <si>
+    <t>maxWidth-large-desktop</t>
+  </si>
+  <si>
+    <t>maxWidth-content</t>
+  </si>
+  <si>
+    <t>font-weight-light</t>
+  </si>
+  <si>
+    <t>font-weight-normal</t>
+  </si>
+  <si>
+    <t>font-weight-medium</t>
+  </si>
+  <si>
+    <t>font-weight-bold</t>
+  </si>
+  <si>
+    <t>font-weight-extra-bold</t>
+  </si>
+  <si>
+    <t>fontWeight-light</t>
+  </si>
+  <si>
+    <t>fontWeight-normal</t>
+  </si>
+  <si>
+    <t>fontWeight-medium</t>
+  </si>
+  <si>
+    <t>fontWeight-bold</t>
+  </si>
+  <si>
+    <t>fontWeight-extra-bold</t>
+  </si>
+  <si>
+    <t>color-text-primary</t>
+  </si>
+  <si>
+    <t>color-text-secondary</t>
+  </si>
+  <si>
+    <t>color-text-attention</t>
+  </si>
+  <si>
+    <t>color-text-subtitle</t>
+  </si>
+  <si>
+    <t>color-text--disabled</t>
+  </si>
+  <si>
+    <t>textColor--disabled</t>
+  </si>
+  <si>
+    <t>color-bg-primary</t>
+  </si>
+  <si>
+    <t>color-bg-secondary</t>
+  </si>
+  <si>
+    <t>color-bg-attention</t>
+  </si>
+  <si>
+    <t>color-bg-subtitle</t>
+  </si>
+  <si>
+    <t>color-bg--disabled</t>
+  </si>
+  <si>
+    <t>backgroundColor-primary</t>
+  </si>
+  <si>
+    <t>backgroundColor-secondary</t>
+  </si>
+  <si>
+    <t>backgroundColor-attention</t>
+  </si>
+  <si>
+    <t>backgroundColor-subtitle</t>
+  </si>
+  <si>
+    <t>backgroundColor--disabled</t>
+  </si>
+  <si>
+    <t>lineHeight-none</t>
+  </si>
+  <si>
+    <t>lineHeight-tight</t>
+  </si>
+  <si>
+    <t>lineHeight-snug</t>
+  </si>
+  <si>
+    <t>lineHeight-normal</t>
+  </si>
+  <si>
+    <t>lineHeight-relaxed</t>
+  </si>
+  <si>
+    <t>lineHeight-loose</t>
+  </si>
+  <si>
+    <t>line-height-none</t>
+  </si>
+  <si>
+    <t>line-height-tight</t>
+  </si>
+  <si>
+    <t>line-height-snug</t>
+  </si>
+  <si>
+    <t>line-height-normal</t>
+  </si>
+  <si>
+    <t>line-height-relaxed</t>
+  </si>
+  <si>
+    <t>line-height-loose</t>
+  </si>
+  <si>
+    <t>fontFamily-sans-serif</t>
+  </si>
+  <si>
+    <t>font-family-sans-serif</t>
+  </si>
+  <si>
+    <t>fontFamily-monospace</t>
+  </si>
+  <si>
+    <t>font-family-monospace</t>
+  </si>
+  <si>
+    <t>outlineColor--focus</t>
+  </si>
+  <si>
+    <t>outlineWidth--focus</t>
+  </si>
+  <si>
+    <t>outlineStyle--focus</t>
+  </si>
+  <si>
+    <t>outlineOffset--focus</t>
+  </si>
+  <si>
+    <t>color-outline--focus</t>
+  </si>
+  <si>
+    <t>thickness-outline--focus</t>
+  </si>
+  <si>
+    <t>style-outline--focus</t>
+  </si>
+  <si>
+    <t>offset-outline--focus</t>
+  </si>
+  <si>
+    <t>fontSize-gigantic</t>
+  </si>
+  <si>
+    <t>fontSize-large</t>
+  </si>
+  <si>
+    <t>fontSize-medium</t>
+  </si>
+  <si>
+    <t>fontSize-normal</t>
+  </si>
+  <si>
+    <t>fontSize-small</t>
+  </si>
+  <si>
+    <t>fontSize-smaller</t>
+  </si>
+  <si>
+    <t>fontSize-tiny</t>
+  </si>
+  <si>
+    <t>font-size-gigantic</t>
+  </si>
+  <si>
+    <t>font-size-large</t>
+  </si>
+  <si>
+    <t>font-size-medium</t>
+  </si>
+  <si>
+    <t>font-size-normal</t>
+  </si>
+  <si>
+    <t>font-size-small</t>
+  </si>
+  <si>
+    <t>font-size-smaller</t>
+  </si>
+  <si>
+    <t>font-size-tiny</t>
+  </si>
+  <si>
+    <t>boxShadow-md</t>
+  </si>
+  <si>
+    <t>boxShadow-xl</t>
+  </si>
+  <si>
+    <t>boxShadow-xxl</t>
+  </si>
+  <si>
+    <t>boxShadow-spread</t>
+  </si>
+  <si>
+    <t>boxShadow-spread-2</t>
+  </si>
+  <si>
+    <t>boxShadow-spread-2-xl</t>
+  </si>
+  <si>
+    <t>shadow-md</t>
+  </si>
+  <si>
+    <t>shadow-xl</t>
+  </si>
+  <si>
+    <t>shadow-xxl</t>
+  </si>
+  <si>
+    <t>shadow-spread</t>
+  </si>
+  <si>
+    <t>shadow-spread-2</t>
+  </si>
+  <si>
+    <t>shadow-spread-2-xl</t>
+  </si>
+  <si>
+    <t>backgroundColor-overlay</t>
+  </si>
+  <si>
+    <t>backgroundColor-dropdown-item--hover</t>
+  </si>
+  <si>
+    <t>backgroundColor-dropdown-item--active</t>
+  </si>
+  <si>
+    <t>backgroundColor-dropdown-item--active-hover</t>
+  </si>
+  <si>
+    <t>backgroundColor-tree-row--selected--before</t>
+  </si>
+  <si>
+    <t>borderColor--disabled</t>
+  </si>
+  <si>
+    <t>borderColor-dropdown-item</t>
+  </si>
+  <si>
+    <t>olor-bg-overlay</t>
+  </si>
+  <si>
+    <t>color-bg-dropdown-item--hover</t>
+  </si>
+  <si>
+    <t>color-bg-dropdown-item--active</t>
+  </si>
+  <si>
+    <t>color-bg-dropdown-item--active-hover</t>
+  </si>
+  <si>
+    <t>color-bg-tree-row--selected--before</t>
+  </si>
+  <si>
+    <t>color-border--disabled</t>
+  </si>
+  <si>
+    <t>color-border-dropdown-item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1075,11 +1137,17 @@
       <scheme val="major"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Aptos Display"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1108,12 +1176,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1448,10 +1517,1163 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
+  <dimension ref="A1:C141"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="58.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>144</v>
+      </c>
+      <c r="B24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>184</v>
+      </c>
+      <c r="B26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>251</v>
+      </c>
+      <c r="B51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>174</v>
+      </c>
+      <c r="B52" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>252</v>
+      </c>
+      <c r="B53" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>212</v>
+      </c>
+      <c r="B54" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>213</v>
+      </c>
+      <c r="B55" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>214</v>
+      </c>
+      <c r="B56" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>229</v>
+      </c>
+      <c r="B58" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>228</v>
+      </c>
+      <c r="B59" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>227</v>
+      </c>
+      <c r="B60" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>172</v>
+      </c>
+      <c r="B61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>235</v>
+      </c>
+      <c r="B62" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>234</v>
+      </c>
+      <c r="B63" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>233</v>
+      </c>
+      <c r="B64" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>173</v>
+      </c>
+      <c r="B65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1562,13 +2784,13 @@
         <v>63</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>261</v>
+        <v>209</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>264</v>
+        <v>212</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>267</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1579,13 +2801,13 @@
         <v>63</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>262</v>
+        <v>210</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>265</v>
+        <v>213</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>268</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1596,13 +2818,13 @@
         <v>63</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>263</v>
+        <v>211</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>266</v>
+        <v>214</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>269</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1653,10 +2875,10 @@
         <v>63</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>283</v>
+        <v>227</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>286</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1670,10 +2892,10 @@
         <v>63</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>284</v>
+        <v>228</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>287</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1687,10 +2909,10 @@
         <v>63</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>285</v>
+        <v>229</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>288</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1718,13 +2940,13 @@
         <v>63</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>249</v>
+        <v>197</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>243</v>
+        <v>191</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>244</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1735,13 +2957,13 @@
         <v>63</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>245</v>
+        <v>193</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>246</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1752,13 +2974,13 @@
         <v>63</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>247</v>
+        <v>195</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>248</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1786,13 +3008,13 @@
         <v>63</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>250</v>
+        <v>198</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>255</v>
+        <v>203</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>258</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1803,13 +3025,13 @@
         <v>63</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>253</v>
+        <v>201</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>259</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1820,13 +3042,13 @@
         <v>63</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>254</v>
+        <v>202</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>257</v>
+        <v>205</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>260</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1888,13 +3110,13 @@
         <v>63</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>270</v>
+        <v>218</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>273</v>
+        <v>221</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>276</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1905,13 +3127,13 @@
         <v>63</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>271</v>
+        <v>219</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>274</v>
+        <v>222</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>277</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1922,13 +3144,13 @@
         <v>63</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>272</v>
+        <v>220</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>275</v>
+        <v>223</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>278</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1962,10 +3184,10 @@
         <v>63</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>289</v>
+        <v>233</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>292</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1979,10 +3201,10 @@
         <v>63</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>290</v>
+        <v>234</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>293</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1996,10 +3218,10 @@
         <v>63</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>291</v>
+        <v>235</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>294</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -2521,7 +3743,7 @@
         <v>156</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>139</v>
@@ -2887,7 +4109,7 @@
         <v>154</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -3082,540 +4304,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A87"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="58.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114F83F-F3AF-0B4F-A4C1-A92AE23C196B}">
-  <dimension ref="A1:A13"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>331</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
build: prepare to release v0.8.0 (#909)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1F8C3A-9F6A-EA4A-A5D8-A6FA8B6AAA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEEB7A1-6D8E-D84D-9BFB-F5A9AE3A6C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" activeTab="1" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Layout and Theme vars" sheetId="3" r:id="rId1"/>
-    <sheet name="Changelog" sheetId="4" r:id="rId2"/>
-    <sheet name="More to rename" sheetId="5" r:id="rId3"/>
+    <sheet name="Changelog" sheetId="4" r:id="rId1"/>
+    <sheet name="Layout and Theme vars" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="353">
   <si>
     <t>width</t>
   </si>
@@ -589,144 +588,12 @@
     <t>scroll-vertical</t>
   </si>
   <si>
-    <t>Introduce borderHorizontal</t>
-  </si>
-  <si>
-    <t>Introduce borderVertical</t>
-  </si>
-  <si>
-    <t>italic --&gt; fontStyle</t>
-  </si>
-  <si>
-    <t>shadow --&gt; boxShadow</t>
-  </si>
-  <si>
-    <t>borderThickness --&gt; borderWidth</t>
-  </si>
-  <si>
-    <t>horizontalMargin --&gt; marginHorizontal</t>
-  </si>
-  <si>
-    <t>verticalMargin --&gt; marginVertical</t>
-  </si>
-  <si>
-    <t>horizontalPadding --&gt; paddingHorizontal</t>
-  </si>
-  <si>
-    <t>verticalPadding --&gt; paddingVertical</t>
-  </si>
-  <si>
     <t>(existing theme vars: offset-decoration)</t>
   </si>
   <si>
-    <t>offset-decoration --&gt; textUnderlineOffset</t>
-  </si>
-  <si>
-    <t>text-transform --&gt; textTransform</t>
-  </si>
-  <si>
-    <t>transform-text --&gt; textTransform</t>
-  </si>
-  <si>
-    <t>"transform-" --&gt; textTransform</t>
-  </si>
-  <si>
-    <t>thickness-decoration --&gt; textDecorationThickness</t>
-  </si>
-  <si>
-    <t>style-decoration --&gt; textDecorationStyle</t>
-  </si>
-  <si>
-    <t>line-decoration --&gt; textDecorationLine</t>
-  </si>
-  <si>
-    <t>color-decoration --&gt; textDecorationColor</t>
-  </si>
-  <si>
-    <t>text-decoration --&gt; textDecoration</t>
-  </si>
-  <si>
-    <t>Changes (layout properties)</t>
-  </si>
-  <si>
-    <t>Changes (theme variables)</t>
-  </si>
-  <si>
-    <t>color-outline --&gt; outlineColor</t>
-  </si>
-  <si>
-    <t>offset-outline --&gt; outlineOffset</t>
-  </si>
-  <si>
-    <t>style-outline --&gt; outlineStyle</t>
-  </si>
-  <si>
     <t>thickness-outline</t>
   </si>
   <si>
-    <t>thickness-outline --&gt; outlineWidth</t>
-  </si>
-  <si>
-    <t>letter-spacing --&gt; letterSpacing</t>
-  </si>
-  <si>
-    <t>line-height --&gt; lineHeight</t>
-  </si>
-  <si>
-    <t>font-family --&gt; fontFamily</t>
-  </si>
-  <si>
-    <t>font-size --&gt; fontSize</t>
-  </si>
-  <si>
-    <t>font-style --&gt; fontStyle</t>
-  </si>
-  <si>
-    <t>margin-horizontal --&gt; marginHorizontal</t>
-  </si>
-  <si>
-    <t>margin-vertical --&gt; marginVertical</t>
-  </si>
-  <si>
-    <t>scroll-horizontal --&gt; overflowX</t>
-  </si>
-  <si>
-    <t>scroll-vertical --&gt; overflowY</t>
-  </si>
-  <si>
-    <t>padding-horizontal --&gt; paddingHorizontal</t>
-  </si>
-  <si>
-    <t>padding-vertical --&gt; paddingVertical</t>
-  </si>
-  <si>
-    <t>padding-bottom --&gt; paddingBottom</t>
-  </si>
-  <si>
-    <t>padding-right --&gt; paddingRight</t>
-  </si>
-  <si>
-    <t>padding-left --&gt; paddingLeft</t>
-  </si>
-  <si>
-    <t>padding-top --&gt; paddingTop</t>
-  </si>
-  <si>
-    <t>margin-bottom --&gt; marginBottom</t>
-  </si>
-  <si>
-    <t>margin-left --&gt; marginLeft</t>
-  </si>
-  <si>
-    <t>margin-right --&gt; marginRight</t>
-  </si>
-  <si>
-    <t>margin-top --&gt; marginTop</t>
-  </si>
-  <si>
-    <t>min-width --&gt; minWidth</t>
-  </si>
-  <si>
     <t>media-maxWidth-phone</t>
   </si>
   <si>
@@ -745,30 +612,6 @@
     <t>max-content-width</t>
   </si>
   <si>
-    <t>max-width --&gt; maxWidth</t>
-  </si>
-  <si>
-    <t>max-height --&gt; maxHeight</t>
-  </si>
-  <si>
-    <t>min-height --&gt; minHeight</t>
-  </si>
-  <si>
-    <t>radius --&gt; borderRadius</t>
-  </si>
-  <si>
-    <t>border-radius-end-start --&gt; borderRadiusEndStart</t>
-  </si>
-  <si>
-    <t>border-radius-end-end --&gt; borderRadiusEndEnd</t>
-  </si>
-  <si>
-    <t>border-radius-start-start --&gt; borderRadiusStartStart</t>
-  </si>
-  <si>
-    <t>border-radius-start-end --&gt; borderRadiusStartEnd</t>
-  </si>
-  <si>
     <t>color-border-left</t>
   </si>
   <si>
@@ -877,18 +720,6 @@
     <t>borderTopWidth</t>
   </si>
   <si>
-    <t>color-border-bottom --&gt; borderBottomColor</t>
-  </si>
-  <si>
-    <t>style-border-bottom --&gt; borderBottomStyle</t>
-  </si>
-  <si>
-    <t>thickness-border-bottom --&gt; borderBottomThickness</t>
-  </si>
-  <si>
-    <t>border-bottom --&gt; borderBottom</t>
-  </si>
-  <si>
     <t>color-border-horizontal</t>
   </si>
   <si>
@@ -925,102 +756,6 @@
     <t>borderVerticalWidth</t>
   </si>
   <si>
-    <t>thickness-border-horizontal --&gt; borderHorizontalWidth</t>
-  </si>
-  <si>
-    <t>style-border-horizontal --&gt; borderHorizontalStyle</t>
-  </si>
-  <si>
-    <t>color-border-horizontal --&gt; borderHorizontalColor</t>
-  </si>
-  <si>
-    <t>border-horizontal --&gt; borderHorizontal</t>
-  </si>
-  <si>
-    <t>thickness-border-vertical --&gt; borderVerticalWidth</t>
-  </si>
-  <si>
-    <t>style-border-vertical --&gt; borderVerticalStyle</t>
-  </si>
-  <si>
-    <t>color-border-vertical --&gt; borderVerticalColor</t>
-  </si>
-  <si>
-    <t>border-vertical --&gt; borderVertical</t>
-  </si>
-  <si>
-    <t>thickness-border-left --&gt; borderLeftWidth</t>
-  </si>
-  <si>
-    <t>style-border-left --&gt; borderLeftStyle</t>
-  </si>
-  <si>
-    <t>color-border-left --&gt; borderLeftColor</t>
-  </si>
-  <si>
-    <t>border-left --&gt; borderLeft</t>
-  </si>
-  <si>
-    <t>thickness-border-right --&gt; borderRightWidth</t>
-  </si>
-  <si>
-    <t>style-border-right --&gt; borderRigthStyle</t>
-  </si>
-  <si>
-    <t>color-border-right --&gt; borderRigthColor</t>
-  </si>
-  <si>
-    <t>border-right --&gt; borderRigth</t>
-  </si>
-  <si>
-    <t>thickness-border-top --&gt; borderTopWidth</t>
-  </si>
-  <si>
-    <t>style-border-top --&gt; borderTopStyle</t>
-  </si>
-  <si>
-    <t>color-border-top --&gt; borderTopColor</t>
-  </si>
-  <si>
-    <t>border-top --&gt; borderTop</t>
-  </si>
-  <si>
-    <t>thickness-border --&gt; borderWidth</t>
-  </si>
-  <si>
-    <t>style-border --&gt; borderStyle</t>
-  </si>
-  <si>
-    <t>color-text: review</t>
-  </si>
-  <si>
-    <t>color-border --&gt; borderColor</t>
-  </si>
-  <si>
-    <t>color-bg --&gt; backgroundColor</t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
-    <t>media-maxWidth-phone --&gt; maxWidth-phone</t>
-  </si>
-  <si>
-    <t>media-maxWidth-landscape-phone --&gt; maxWidth-landscape-phone</t>
-  </si>
-  <si>
-    <t>media-maxWidth-tablet --&gt; maxWidth-tablet</t>
-  </si>
-  <si>
-    <t>media-maxWidth-desktop --&gt; maxWidth-desktop</t>
-  </si>
-  <si>
-    <t>media-maxWidth-large-desktop --&gt; maxWidth-large-desktop</t>
-  </si>
-  <si>
-    <t>max-content-width --&gt; maxWidth-content</t>
-  </si>
-  <si>
     <t>textColor-primary</t>
   </si>
   <si>
@@ -1033,14 +768,341 @@
     <t>textColor-secondary</t>
   </si>
   <si>
-    <t>shadow-md --&gt; boxShadow-md</t>
+    <t>Old name</t>
+  </si>
+  <si>
+    <t>New name</t>
+  </si>
+  <si>
+    <t>Layout (inline component) properties</t>
+  </si>
+  <si>
+    <t>Theme variable prefixes</t>
+  </si>
+  <si>
+    <t>App-bound theme variables</t>
+  </si>
+  <si>
+    <t>boolean changed to "normal" or "italic"</t>
+  </si>
+  <si>
+    <t>transform-text</t>
+  </si>
+  <si>
+    <t>transform</t>
+  </si>
+  <si>
+    <t>border-radius-end-end</t>
+  </si>
+  <si>
+    <t>border-radius-start-end</t>
+  </si>
+  <si>
+    <t>borderBottomThickness</t>
+  </si>
+  <si>
+    <t>borderRigthStyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> borderRigthColor</t>
+  </si>
+  <si>
+    <t>borderRigth</t>
+  </si>
+  <si>
+    <t>maxWidth-phone</t>
+  </si>
+  <si>
+    <t>maxWidth-landscape-phone</t>
+  </si>
+  <si>
+    <t>maxWidth-tablet</t>
+  </si>
+  <si>
+    <t>maxWidth-desktop</t>
+  </si>
+  <si>
+    <t>maxWidth-large-desktop</t>
+  </si>
+  <si>
+    <t>maxWidth-content</t>
+  </si>
+  <si>
+    <t>font-weight-light</t>
+  </si>
+  <si>
+    <t>font-weight-normal</t>
+  </si>
+  <si>
+    <t>font-weight-medium</t>
+  </si>
+  <si>
+    <t>font-weight-bold</t>
+  </si>
+  <si>
+    <t>font-weight-extra-bold</t>
+  </si>
+  <si>
+    <t>fontWeight-light</t>
+  </si>
+  <si>
+    <t>fontWeight-normal</t>
+  </si>
+  <si>
+    <t>fontWeight-medium</t>
+  </si>
+  <si>
+    <t>fontWeight-bold</t>
+  </si>
+  <si>
+    <t>fontWeight-extra-bold</t>
+  </si>
+  <si>
+    <t>color-text-primary</t>
+  </si>
+  <si>
+    <t>color-text-secondary</t>
+  </si>
+  <si>
+    <t>color-text-attention</t>
+  </si>
+  <si>
+    <t>color-text-subtitle</t>
+  </si>
+  <si>
+    <t>color-text--disabled</t>
+  </si>
+  <si>
+    <t>textColor--disabled</t>
+  </si>
+  <si>
+    <t>color-bg-primary</t>
+  </si>
+  <si>
+    <t>color-bg-secondary</t>
+  </si>
+  <si>
+    <t>color-bg-attention</t>
+  </si>
+  <si>
+    <t>color-bg-subtitle</t>
+  </si>
+  <si>
+    <t>color-bg--disabled</t>
+  </si>
+  <si>
+    <t>backgroundColor-primary</t>
+  </si>
+  <si>
+    <t>backgroundColor-secondary</t>
+  </si>
+  <si>
+    <t>backgroundColor-attention</t>
+  </si>
+  <si>
+    <t>backgroundColor-subtitle</t>
+  </si>
+  <si>
+    <t>backgroundColor--disabled</t>
+  </si>
+  <si>
+    <t>lineHeight-none</t>
+  </si>
+  <si>
+    <t>lineHeight-tight</t>
+  </si>
+  <si>
+    <t>lineHeight-snug</t>
+  </si>
+  <si>
+    <t>lineHeight-normal</t>
+  </si>
+  <si>
+    <t>lineHeight-relaxed</t>
+  </si>
+  <si>
+    <t>lineHeight-loose</t>
+  </si>
+  <si>
+    <t>line-height-none</t>
+  </si>
+  <si>
+    <t>line-height-tight</t>
+  </si>
+  <si>
+    <t>line-height-snug</t>
+  </si>
+  <si>
+    <t>line-height-normal</t>
+  </si>
+  <si>
+    <t>line-height-relaxed</t>
+  </si>
+  <si>
+    <t>line-height-loose</t>
+  </si>
+  <si>
+    <t>fontFamily-sans-serif</t>
+  </si>
+  <si>
+    <t>font-family-sans-serif</t>
+  </si>
+  <si>
+    <t>fontFamily-monospace</t>
+  </si>
+  <si>
+    <t>font-family-monospace</t>
+  </si>
+  <si>
+    <t>outlineColor--focus</t>
+  </si>
+  <si>
+    <t>outlineWidth--focus</t>
+  </si>
+  <si>
+    <t>outlineStyle--focus</t>
+  </si>
+  <si>
+    <t>outlineOffset--focus</t>
+  </si>
+  <si>
+    <t>color-outline--focus</t>
+  </si>
+  <si>
+    <t>thickness-outline--focus</t>
+  </si>
+  <si>
+    <t>style-outline--focus</t>
+  </si>
+  <si>
+    <t>offset-outline--focus</t>
+  </si>
+  <si>
+    <t>fontSize-gigantic</t>
+  </si>
+  <si>
+    <t>fontSize-large</t>
+  </si>
+  <si>
+    <t>fontSize-medium</t>
+  </si>
+  <si>
+    <t>fontSize-normal</t>
+  </si>
+  <si>
+    <t>fontSize-small</t>
+  </si>
+  <si>
+    <t>fontSize-smaller</t>
+  </si>
+  <si>
+    <t>fontSize-tiny</t>
+  </si>
+  <si>
+    <t>font-size-gigantic</t>
+  </si>
+  <si>
+    <t>font-size-large</t>
+  </si>
+  <si>
+    <t>font-size-medium</t>
+  </si>
+  <si>
+    <t>font-size-normal</t>
+  </si>
+  <si>
+    <t>font-size-small</t>
+  </si>
+  <si>
+    <t>font-size-smaller</t>
+  </si>
+  <si>
+    <t>font-size-tiny</t>
+  </si>
+  <si>
+    <t>boxShadow-md</t>
+  </si>
+  <si>
+    <t>boxShadow-xl</t>
+  </si>
+  <si>
+    <t>boxShadow-xxl</t>
+  </si>
+  <si>
+    <t>boxShadow-spread</t>
+  </si>
+  <si>
+    <t>boxShadow-spread-2</t>
+  </si>
+  <si>
+    <t>boxShadow-spread-2-xl</t>
+  </si>
+  <si>
+    <t>shadow-md</t>
+  </si>
+  <si>
+    <t>shadow-xl</t>
+  </si>
+  <si>
+    <t>shadow-xxl</t>
+  </si>
+  <si>
+    <t>shadow-spread</t>
+  </si>
+  <si>
+    <t>shadow-spread-2</t>
+  </si>
+  <si>
+    <t>shadow-spread-2-xl</t>
+  </si>
+  <si>
+    <t>backgroundColor-overlay</t>
+  </si>
+  <si>
+    <t>backgroundColor-dropdown-item--hover</t>
+  </si>
+  <si>
+    <t>backgroundColor-dropdown-item--active</t>
+  </si>
+  <si>
+    <t>backgroundColor-dropdown-item--active-hover</t>
+  </si>
+  <si>
+    <t>backgroundColor-tree-row--selected--before</t>
+  </si>
+  <si>
+    <t>borderColor--disabled</t>
+  </si>
+  <si>
+    <t>borderColor-dropdown-item</t>
+  </si>
+  <si>
+    <t>olor-bg-overlay</t>
+  </si>
+  <si>
+    <t>color-bg-dropdown-item--hover</t>
+  </si>
+  <si>
+    <t>color-bg-dropdown-item--active</t>
+  </si>
+  <si>
+    <t>color-bg-dropdown-item--active-hover</t>
+  </si>
+  <si>
+    <t>color-bg-tree-row--selected--before</t>
+  </si>
+  <si>
+    <t>color-border--disabled</t>
+  </si>
+  <si>
+    <t>color-border-dropdown-item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1075,11 +1137,17 @@
       <scheme val="major"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Aptos Display"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1108,12 +1176,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1448,10 +1517,1163 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
+  <dimension ref="A1:C141"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="58.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>144</v>
+      </c>
+      <c r="B24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>184</v>
+      </c>
+      <c r="B26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>251</v>
+      </c>
+      <c r="B51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>174</v>
+      </c>
+      <c r="B52" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>252</v>
+      </c>
+      <c r="B53" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>212</v>
+      </c>
+      <c r="B54" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>213</v>
+      </c>
+      <c r="B55" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>214</v>
+      </c>
+      <c r="B56" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>229</v>
+      </c>
+      <c r="B58" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>228</v>
+      </c>
+      <c r="B59" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>227</v>
+      </c>
+      <c r="B60" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>172</v>
+      </c>
+      <c r="B61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>235</v>
+      </c>
+      <c r="B62" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>234</v>
+      </c>
+      <c r="B63" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>233</v>
+      </c>
+      <c r="B64" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>173</v>
+      </c>
+      <c r="B65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C990125-402B-AA47-80A8-12F747D62A3D}">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1562,13 +2784,13 @@
         <v>63</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>261</v>
+        <v>209</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>264</v>
+        <v>212</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>267</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1579,13 +2801,13 @@
         <v>63</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>262</v>
+        <v>210</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>265</v>
+        <v>213</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>268</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1596,13 +2818,13 @@
         <v>63</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>263</v>
+        <v>211</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>266</v>
+        <v>214</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>269</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1653,10 +2875,10 @@
         <v>63</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>283</v>
+        <v>227</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>286</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1670,10 +2892,10 @@
         <v>63</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>284</v>
+        <v>228</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>287</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1687,10 +2909,10 @@
         <v>63</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>285</v>
+        <v>229</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>288</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1718,13 +2940,13 @@
         <v>63</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>249</v>
+        <v>197</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>243</v>
+        <v>191</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>244</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1735,13 +2957,13 @@
         <v>63</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>245</v>
+        <v>193</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>246</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1752,13 +2974,13 @@
         <v>63</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>247</v>
+        <v>195</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>248</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1786,13 +3008,13 @@
         <v>63</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>250</v>
+        <v>198</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>255</v>
+        <v>203</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>258</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1803,13 +3025,13 @@
         <v>63</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>253</v>
+        <v>201</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>259</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1820,13 +3042,13 @@
         <v>63</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>254</v>
+        <v>202</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>257</v>
+        <v>205</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>260</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1888,13 +3110,13 @@
         <v>63</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>270</v>
+        <v>218</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>273</v>
+        <v>221</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>276</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1905,13 +3127,13 @@
         <v>63</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>271</v>
+        <v>219</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>274</v>
+        <v>222</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>277</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1922,13 +3144,13 @@
         <v>63</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>272</v>
+        <v>220</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>275</v>
+        <v>223</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>278</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1962,10 +3184,10 @@
         <v>63</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>289</v>
+        <v>233</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>292</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1979,10 +3201,10 @@
         <v>63</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>290</v>
+        <v>234</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>293</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1996,10 +3218,10 @@
         <v>63</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>291</v>
+        <v>235</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>294</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -2521,7 +3743,7 @@
         <v>156</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>139</v>
@@ -2887,7 +4109,7 @@
         <v>154</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -3082,540 +4304,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:A87"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="58.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114F83F-F3AF-0B4F-A4C1-A92AE23C196B}">
-  <dimension ref="A1:A13"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>331</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: fontStretch, fontStyle (#918)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEEB7A1-6D8E-D84D-9BFB-F5A9AE3A6C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BA6375-4109-F048-ADC4-C5DD629C2137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="355">
   <si>
     <t>width</t>
   </si>
@@ -1096,6 +1096,12 @@
   </si>
   <si>
     <t>color-border-dropdown-item</t>
+  </si>
+  <si>
+    <t>font-stretch</t>
+  </si>
+  <si>
+    <t>fontStretch</t>
   </si>
 </sst>
 </file>
@@ -1518,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
-  <dimension ref="A1:C141"/>
+  <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A142" sqref="A142"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2664,6 +2670,14 @@
         <v>345</v>
       </c>
     </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2674,7 +2688,7 @@
   <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat: switching to the new scripting engine (#974)
</commit_message>
<xml_diff>
--- a/xmlui/src/components-core/theming/theme-refactor.xlsx
+++ b/xmlui/src/components-core/theming/theme-refactor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotneteer/source/xmlui/xmlui/src/components-core/theming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BA6375-4109-F048-ADC4-C5DD629C2137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8544D5D3-CC2F-E943-9754-84FD1DA495B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20400" xr2:uid="{6323BA21-4476-9241-87F3-781EB34445EA}"/>
   </bookViews>
@@ -798,9 +798,6 @@
     <t>border-radius-start-end</t>
   </si>
   <si>
-    <t>borderBottomThickness</t>
-  </si>
-  <si>
     <t>borderRigthStyle</t>
   </si>
   <si>
@@ -1065,9 +1062,6 @@
     <t>backgroundColor-dropdown-item--active</t>
   </si>
   <si>
-    <t>backgroundColor-dropdown-item--active-hover</t>
-  </si>
-  <si>
     <t>backgroundColor-tree-row--selected--before</t>
   </si>
   <si>
@@ -1102,6 +1096,12 @@
   </si>
   <si>
     <t>fontStretch</t>
+  </si>
+  <si>
+    <t>borderEndStartRadius</t>
+  </si>
+  <si>
+    <t>backgroundColor-dropdown-item--active--hover</t>
   </si>
 </sst>
 </file>
@@ -1526,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564599AE-A317-F348-A8E0-41DA40D75056}">
   <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1939,7 +1939,7 @@
         <v>176</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>128</v>
+        <v>353</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1987,7 +1987,7 @@
         <v>214</v>
       </c>
       <c r="B56" t="s">
-        <v>253</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -2107,7 +2107,7 @@
         <v>204</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -2115,7 +2115,7 @@
         <v>203</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -2123,7 +2123,7 @@
         <v>70</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -2203,7 +2203,7 @@
         <v>185</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -2211,7 +2211,7 @@
         <v>186</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -2219,7 +2219,7 @@
         <v>187</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -2227,7 +2227,7 @@
         <v>188</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -2235,7 +2235,7 @@
         <v>189</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
@@ -2243,7 +2243,7 @@
         <v>190</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -2256,47 +2256,47 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>239</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>242</v>
@@ -2312,7 +2312,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>240</v>
@@ -2320,7 +2320,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>241</v>
@@ -2328,10 +2328,10 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -2344,106 +2344,106 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -2456,90 +2456,90 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
@@ -2560,90 +2560,90 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>342</v>
+        <v>354</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
@@ -2656,26 +2656,26 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>